<commit_message>
TCs for 4 features
I covered the test cases for :
Add Car
Delete Car
View Car
Search
</commit_message>
<xml_diff>
--- a/5- Testing/Test Cases.xlsx
+++ b/5- Testing/Test Cases.xlsx
@@ -5,20 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beshoy Sameh\Documents\GitHub\Car-Purchasing-App\5- Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Documents\GitHub\Car-Purchasing-App\5- Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2B547F-7C8D-4409-ABD7-D555A4FFA00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1480FA-88A0-4453-AB86-B2AD6C047DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="2" r:id="rId1"/>
     <sheet name="New Customer" sheetId="15" r:id="rId2"/>
     <sheet name="Add Car" sheetId="16" r:id="rId3"/>
     <sheet name="Delete car" sheetId="17" r:id="rId4"/>
-    <sheet name="search" sheetId="18" r:id="rId5"/>
-    <sheet name="View Car" sheetId="19" r:id="rId6"/>
+    <sheet name="View Car" sheetId="19" r:id="rId5"/>
+    <sheet name="search" sheetId="18" r:id="rId6"/>
     <sheet name="login" sheetId="20" r:id="rId7"/>
     <sheet name="Logout" sheetId="21" r:id="rId8"/>
     <sheet name="Regs" sheetId="22" r:id="rId9"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="268">
   <si>
     <t>Module</t>
   </si>
@@ -1928,21 +1928,12 @@
     </r>
   </si>
   <si>
-    <t>sear</t>
-  </si>
-  <si>
-    <t>view car</t>
-  </si>
-  <si>
     <t>lo</t>
   </si>
   <si>
     <t>L</t>
   </si>
   <si>
-    <t>Add Car Functionality for Admin</t>
-  </si>
-  <si>
     <t>TC-AddCar-00</t>
   </si>
   <si>
@@ -1950,14 +1941,6 @@
   </si>
   <si>
     <t>High</t>
-  </si>
-  <si>
-    <t>Verfiy that Admin can add car
-to the system.</t>
-  </si>
-  <si>
-    <t>The car should be displayed 
-in the customer's and admin's home page in addition to that "car added successfullly" meassage is displayed after the car is added.</t>
   </si>
   <si>
     <t>Related  
@@ -1973,27 +1956,9 @@
     <t>General</t>
   </si>
   <si>
-    <t>1. Press "add button" in home page.
-2.  Upload a photo.
-3. Choose " toyota" from brand dropdown list .
-4. Choose  " Toyota " from car model dropdown list.
-5.Fill in "500,000" in the price field.
-6. leave description field blank.
-7. Click on the "Save" button
-8.Verify that the message "Car added successfully" is displayed
-9. Verify that the added car is displayed on the home page</t>
-  </si>
-  <si>
-    <t>An error message should appear 
-          “Please fill out this field.”</t>
-  </si>
-  <si>
     <t>T031, T032</t>
   </si>
   <si>
-    <t>TC-AddCar-02</t>
-  </si>
-  <si>
     <t>Price Field</t>
   </si>
   <si>
@@ -2001,23 +1966,6 @@
   </si>
   <si>
     <t>technical</t>
-  </si>
-  <si>
-    <t>Verfiy that an error message will be displayed for the Admin when the description field left blank.</t>
-  </si>
-  <si>
-    <t>Verfiy that an error message will be displayed for the Admin when the price field left blank.</t>
-  </si>
-  <si>
-    <t>1. Press "add button" in home page.
-2.  Upload a photo.
-3. Choose " toyota" from brand dropdown list .
-4. Choose  " Toyota " from car model dropdown list.
-5.leave the price field blank.
-6. Fill in " Hello " the description field.
-7. Click on the "Save" button
-8.Verify that the message "Car added successfully" is displayed
-9. Verify that the added car is displayed on the home page</t>
   </si>
   <si>
     <t>1- browser is available 
@@ -2043,44 +1991,206 @@
 doesn't accept special charchters.</t>
   </si>
   <si>
-    <t>1. Press "add button" in home page.
+    <t>Verify that a car can be added successfully by an admin.</t>
+  </si>
+  <si>
+    <t>1. The car should be added successfully.
+2. A success message should be displayed indicating that the car has been added "car added successfullly".
+3. The added car should be displayed in the car list on the home page for the admin and customer .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Press "add button" in home page.
 2.  Upload a photo.
 3. Choose " toyota" from brand dropdown list .
 4. Choose  " Toyota " from car model dropdown list.
 5.Fill in "%$## in the price field.
 6. Fill in " Hello " the description field.
 7. Click on the "Save" button
-8.Verify that the message "Car added successfully" is displayed
-9. Verify that the added car is displayed on the home page</t>
-  </si>
-  <si>
-    <t>The price field shoudln't accept 
-special characters.</t>
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. The price field shoudln't accept 
+special characters.
+2. The car should not be added to the car list on the home page.
+</t>
+  </si>
+  <si>
+    <t>Verify that an error message will be displayed for the Admin when the price field is left blank.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Press "add button" in home page.
+2.  Upload a photo.
+3. Choose " toyota" from brand dropdown list .
+4. Choose  " Toyota " from car model dropdown list.
+5.Fill in "  " in the price field.
+6. Fill in " Hello " the description field.
+7. Click on the "Save" button
+</t>
+  </si>
+  <si>
+    <t>1. An error message "Please fill out this field" should be displayed.
+2. The car should not be added to the car list on the home page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Press "add button" in home page.
+2.  Upload a photo.
+3. Choose " toyota" from brand dropdown list .
+4. Choose  " Toyota " from car model dropdown list.
+5.Fill in "500,000" in the price field.
+6.Fill in "  " in description field
+7. Click on the "Save" button
+</t>
+  </si>
+  <si>
+    <t>Verify that an error message will be displayed for the Admin when the description field is left blank.</t>
+  </si>
+  <si>
+    <t>1. An error message "Please fill out this field" should be displayed.
+2. The car should not be added to the car list on the home page.</t>
+  </si>
+  <si>
+    <t>Alternative flow</t>
   </si>
   <si>
     <t>TC-AddCar-
-Price-04</t>
-  </si>
-  <si>
-    <t>1. Press "add button" in home page.
+Cancel-04</t>
+  </si>
+  <si>
+    <t>Verify that an admin can cancel adding a car.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Press "add button" in home page.
 2.  Upload a photo.
 3. Choose " toyota" from brand dropdown list .
 4. Choose  " Toyota " from car model dropdown list.
 5.Fill in "500,000" in the price field.
 6. Fill in " Hello " in the description field.
 7. Click on the "Save" button
-8.Verify that the message "Car added successfully" is displayed
-9. Verify that the added car is displayed on the home page</t>
-  </si>
-  <si>
-    <t>REQ-6.1</t>
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Press "add button" in home page.
+2.  Upload a photo.
+3. Choose " toyota" from brand dropdown list .
+4. Choose  " Toyota " from car model dropdown list.
+5.Fill in "500,000" in the price field.
+6. Fill in " Hello " in the description field.
+7. Click on the "Cancel" button
+</t>
+  </si>
+  <si>
+    <t>1. The home page should be
+ displayed.
+2. The car should not be added to the car list on the home page.</t>
+  </si>
+  <si>
+    <t>TC-DelCar-00</t>
+  </si>
+  <si>
+    <t>REQ-7</t>
+  </si>
+  <si>
+    <t>Verify that an admin can delete a car successfully</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Choose one of the available cars on the home page.
+2. Click on the "Delete" button for that car.
+</t>
+  </si>
+  <si>
+    <t>1. The car should be deleted successfully.
+2. A success message should be displayed in new page indicating that the car has been deleted successfully "Car is deleted successfully in new page".
+3. The deleted car should not be displayed in the car list on the home page for admin and user.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer </t>
+  </si>
+  <si>
+    <t>TC-AddCar-
+User-04</t>
+  </si>
+  <si>
+    <t>1- browser is available 
+2- Login as user successfully</t>
+  </si>
+  <si>
+    <t>verify that the car has been added to the user successfully to his home page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- browser is available 
+</t>
+  </si>
+  <si>
+    <t>1. Open the login page.
+2. Fill in :salma@gmail.com" in email field.
+3. Fill in " *********" in the password field 
+4.Click on the "Login" button.
+5. Check that the car is added to the home page.</t>
+  </si>
+  <si>
+    <t>The car with its details, that the admin already added, should be displayed on the user's home page.</t>
+  </si>
+  <si>
+    <t>TC-DelCar-
+User-04</t>
+  </si>
+  <si>
+    <t>verify that the car has been deleted from the user's home page.</t>
+  </si>
+  <si>
+    <t>The car with its details, that the admin already added, should be deleted from the user's home page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the login page.
+2. Fill in :salma@gmail.com" in email field.
+3. Fill in " *********" in the password field 
+4.Click on the "Login" button.
+5. Check that the car is deleted from the home page.
+</t>
+  </si>
+  <si>
+    <t>REQ-4</t>
+  </si>
+  <si>
+    <t>TC-HomePage-00</t>
+  </si>
+  <si>
+    <t>Verify that the Home Page displays all unreserved cars in the database with their details and reserve button.</t>
+  </si>
+  <si>
+    <t>1.Check that all unreserved cars in the database are displayed on the home page.
+2. Verify that the following information is displayed for each car: photo, price, brand, model, description, and reserve button.</t>
+  </si>
+  <si>
+    <t>All unreserved cars in the database are displayed on the Home Page with their details and reserve button below each one.</t>
+  </si>
+  <si>
+    <t>REQ-5</t>
+  </si>
+  <si>
+    <t>Verify if the user can search for cars by  brand name.</t>
+  </si>
+  <si>
+    <t>1. Click on the search bar.
+2. Enter "toyota " in the search bar.
+3. Click on the search button.
+.</t>
+  </si>
+  <si>
+    <t>The system should display a list of cars that match the toyota brand.</t>
+  </si>
+  <si>
+    <t>TC-SearchBrand-00</t>
+  </si>
+  <si>
+    <t>Verify that user sees a pop-up message when there are no cars available for the entered brand name.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2166,12 +2276,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="2"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -2198,8 +2302,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF374151"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="35">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2340,48 +2464,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor rgb="FF6FA8DC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor rgb="FF3D85C6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor rgb="FF0B5394"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor rgb="FF073763"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor rgb="FF351C75"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor rgb="FF20124D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.34998626667073579"/>
         <bgColor rgb="FF4C1130"/>
       </patternFill>
@@ -2405,7 +2487,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -2465,11 +2547,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2561,6 +2695,33 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2587,72 +2748,77 @@
     <xf numFmtId="0" fontId="11" fillId="22" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="26" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6478,7 +6644,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="140.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="40" t="s">
         <v>57</v>
       </c>
       <c r="B2" s="21" t="s">
@@ -6525,8 +6691,8 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="147" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="32"/>
-      <c r="B3" s="34" t="s">
+      <c r="A3" s="41"/>
+      <c r="B3" s="43" t="s">
         <v>69</v>
       </c>
       <c r="C3" s="22" t="s">
@@ -6570,8 +6736,8 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="138.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="32"/>
-      <c r="B4" s="32"/>
+      <c r="A4" s="41"/>
+      <c r="B4" s="41"/>
       <c r="C4" s="22" t="s">
         <v>76</v>
       </c>
@@ -6613,8 +6779,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="32"/>
-      <c r="B5" s="32"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="41"/>
       <c r="C5" s="22" t="s">
         <v>80</v>
       </c>
@@ -6656,8 +6822,8 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="145.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="32"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="42"/>
       <c r="C6" s="22" t="s">
         <v>84</v>
       </c>
@@ -6699,8 +6865,8 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="138" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="32"/>
-      <c r="B7" s="35" t="s">
+      <c r="A7" s="41"/>
+      <c r="B7" s="44" t="s">
         <v>89</v>
       </c>
       <c r="C7" s="22" t="s">
@@ -6744,8 +6910,8 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="145.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
+      <c r="A8" s="41"/>
+      <c r="B8" s="41"/>
       <c r="C8" s="22" t="s">
         <v>94</v>
       </c>
@@ -6787,8 +6953,8 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="145.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="32"/>
-      <c r="B9" s="33"/>
+      <c r="A9" s="41"/>
+      <c r="B9" s="42"/>
       <c r="C9" s="22" t="s">
         <v>97</v>
       </c>
@@ -6830,8 +6996,8 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="32"/>
-      <c r="B10" s="36" t="s">
+      <c r="A10" s="41"/>
+      <c r="B10" s="45" t="s">
         <v>101</v>
       </c>
       <c r="C10" s="22" t="s">
@@ -6875,8 +7041,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="32"/>
-      <c r="B11" s="32"/>
+      <c r="A11" s="41"/>
+      <c r="B11" s="41"/>
       <c r="C11" s="22" t="s">
         <v>106</v>
       </c>
@@ -6918,8 +7084,8 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="41"/>
       <c r="C12" s="22" t="s">
         <v>110</v>
       </c>
@@ -6961,8 +7127,8 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="42"/>
       <c r="C13" s="22" t="s">
         <v>115</v>
       </c>
@@ -7004,8 +7170,8 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="32"/>
-      <c r="B14" s="37" t="s">
+      <c r="A14" s="41"/>
+      <c r="B14" s="46" t="s">
         <v>119</v>
       </c>
       <c r="C14" s="22" t="s">
@@ -7049,8 +7215,8 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
+      <c r="A15" s="41"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="22" t="s">
         <v>124</v>
       </c>
@@ -7092,8 +7258,8 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="32"/>
-      <c r="B16" s="32"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="22" t="s">
         <v>128</v>
       </c>
@@ -7135,8 +7301,8 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="32"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="41"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="22" t="s">
         <v>133</v>
       </c>
@@ -7178,8 +7344,8 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="32"/>
-      <c r="B18" s="38" t="s">
+      <c r="A18" s="41"/>
+      <c r="B18" s="47" t="s">
         <v>137</v>
       </c>
       <c r="C18" s="22" t="s">
@@ -7223,8 +7389,8 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="32"/>
-      <c r="B19" s="32"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="22" t="s">
         <v>142</v>
       </c>
@@ -7266,8 +7432,8 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="32"/>
-      <c r="B20" s="32"/>
+      <c r="A20" s="41"/>
+      <c r="B20" s="41"/>
       <c r="C20" s="22" t="s">
         <v>146</v>
       </c>
@@ -7309,8 +7475,8 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="32"/>
-      <c r="B21" s="32"/>
+      <c r="A21" s="41"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="22" t="s">
         <v>151</v>
       </c>
@@ -7352,8 +7518,8 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="32"/>
-      <c r="B22" s="32"/>
+      <c r="A22" s="41"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="22" t="s">
         <v>156</v>
       </c>
@@ -7395,8 +7561,8 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="32"/>
-      <c r="B23" s="33"/>
+      <c r="A23" s="41"/>
+      <c r="B23" s="42"/>
       <c r="C23" s="22" t="s">
         <v>161</v>
       </c>
@@ -7438,8 +7604,8 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="32"/>
-      <c r="B24" s="39" t="s">
+      <c r="A24" s="41"/>
+      <c r="B24" s="48" t="s">
         <v>165</v>
       </c>
       <c r="C24" s="22" t="s">
@@ -7483,8 +7649,8 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="32"/>
-      <c r="B25" s="32"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="41"/>
       <c r="C25" s="22" t="s">
         <v>170</v>
       </c>
@@ -7526,8 +7692,8 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="32"/>
-      <c r="B26" s="32"/>
+      <c r="A26" s="41"/>
+      <c r="B26" s="41"/>
       <c r="C26" s="22" t="s">
         <v>174</v>
       </c>
@@ -7569,8 +7735,8 @@
       </c>
     </row>
     <row r="27" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="32"/>
-      <c r="B27" s="33"/>
+      <c r="A27" s="41"/>
+      <c r="B27" s="42"/>
       <c r="C27" s="22" t="s">
         <v>179</v>
       </c>
@@ -7612,8 +7778,8 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="32"/>
-      <c r="B28" s="40" t="s">
+      <c r="A28" s="41"/>
+      <c r="B28" s="49" t="s">
         <v>183</v>
       </c>
       <c r="C28" s="22" t="s">
@@ -7657,8 +7823,8 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="32"/>
-      <c r="B29" s="32"/>
+      <c r="A29" s="41"/>
+      <c r="B29" s="41"/>
       <c r="C29" s="22" t="s">
         <v>189</v>
       </c>
@@ -7700,8 +7866,8 @@
       </c>
     </row>
     <row r="30" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="32"/>
-      <c r="B30" s="32"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="41"/>
       <c r="C30" s="22" t="s">
         <v>193</v>
       </c>
@@ -7743,8 +7909,8 @@
       </c>
     </row>
     <row r="31" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="33"/>
-      <c r="B31" s="33"/>
+      <c r="A31" s="42"/>
+      <c r="B31" s="42"/>
       <c r="C31" s="22" t="s">
         <v>197</v>
       </c>
@@ -7802,10 +7968,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7E3B47-1521-4401-9600-50F8B310637B}">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7813,1321 +7979,913 @@
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="5" width="30.85546875" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="33.42578125" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" customWidth="1"/>
+    <col min="8" max="8" width="40.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="34.28515625" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" customWidth="1"/>
+    <col min="12" max="12" width="24.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="61" t="s">
-        <v>216</v>
-      </c>
-      <c r="E1" s="55" t="s">
+      <c r="D1" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="55" t="s">
+      <c r="G1" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="55" t="s">
+      <c r="H1" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="55" t="s">
+      <c r="I1" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="55" t="s">
+      <c r="J1" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="K1" s="55" t="s">
+      <c r="K1" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="L1" s="55" t="s">
+      <c r="L1" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="M1" s="55" t="s">
+      <c r="M1" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="N1" s="55" t="s">
+      <c r="N1" s="34" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="249.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="51" t="s">
-        <v>210</v>
-      </c>
-      <c r="B2" s="54" t="s">
-        <v>219</v>
-      </c>
-      <c r="C2" s="56" t="s">
-        <v>211</v>
-      </c>
-      <c r="D2" s="60" t="s">
-        <v>217</v>
-      </c>
-      <c r="E2" s="57" t="s">
+    <row r="2" spans="1:14" ht="207" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="50"/>
+      <c r="B2" s="33" t="s">
         <v>214</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>225</v>
       </c>
       <c r="F2" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="G2" s="58" t="s">
+      <c r="G2" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="J2" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="K2" s="56" t="s">
+        <v>226</v>
+      </c>
+      <c r="L2" s="36"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="32"/>
+    </row>
+    <row r="3" spans="1:14" ht="175.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="51"/>
+      <c r="B3" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>233</v>
+      </c>
+      <c r="F3" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>232</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="J3" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="K3" s="57" t="s">
+        <v>234</v>
+      </c>
+      <c r="L3" s="30"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="32"/>
+    </row>
+    <row r="4" spans="1:14" ht="142.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="51"/>
+      <c r="B4" s="53" t="s">
+        <v>216</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>222</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>217</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>229</v>
+      </c>
+      <c r="F4" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="H4" s="36" t="s">
         <v>230</v>
       </c>
-      <c r="H2" s="58" t="s">
-        <v>239</v>
-      </c>
-      <c r="I2" s="59" t="s">
-        <v>212</v>
-      </c>
-      <c r="J2" s="59" t="s">
-        <v>213</v>
-      </c>
-      <c r="K2" s="57" t="s">
-        <v>215</v>
-      </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="42"/>
-    </row>
-    <row r="3" spans="1:14" ht="262.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="52"/>
-      <c r="B3" s="54" t="s">
-        <v>218</v>
-      </c>
-      <c r="C3" s="60" t="s">
-        <v>232</v>
-      </c>
-      <c r="D3" s="56" t="s">
-        <v>222</v>
-      </c>
-      <c r="E3" s="57" t="s">
-        <v>227</v>
-      </c>
-      <c r="F3" s="59" t="s">
-        <v>226</v>
-      </c>
-      <c r="G3" s="58" t="s">
-        <v>230</v>
-      </c>
-      <c r="H3" s="58" t="s">
-        <v>220</v>
-      </c>
-      <c r="I3" s="59" t="s">
-        <v>212</v>
-      </c>
-      <c r="J3" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K3" s="62" t="s">
-        <v>221</v>
-      </c>
-      <c r="L3" s="30"/>
-      <c r="M3" s="41"/>
-      <c r="N3" s="42"/>
-    </row>
-    <row r="4" spans="1:14" ht="242.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="52"/>
-      <c r="B4" s="63" t="s">
-        <v>224</v>
-      </c>
-      <c r="C4" s="60" t="s">
-        <v>233</v>
-      </c>
-      <c r="D4" s="56" t="s">
-        <v>225</v>
-      </c>
-      <c r="E4" s="57" t="s">
-        <v>228</v>
-      </c>
-      <c r="F4" s="59" t="s">
-        <v>226</v>
-      </c>
-      <c r="G4" s="58" t="s">
-        <v>230</v>
-      </c>
-      <c r="H4" s="58" t="s">
-        <v>229</v>
-      </c>
-      <c r="I4" s="59" t="s">
-        <v>212</v>
-      </c>
-      <c r="J4" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K4" s="62" t="s">
-        <v>221</v>
+      <c r="I4" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="J4" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="K4" s="57" t="s">
+        <v>231</v>
       </c>
       <c r="L4" s="23"/>
       <c r="M4" s="25"/>
-      <c r="N4" s="42"/>
-    </row>
-    <row r="5" spans="1:14" ht="256.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="52"/>
-      <c r="B5" s="65"/>
-      <c r="C5" s="60" t="s">
-        <v>234</v>
-      </c>
-      <c r="D5" s="56" t="s">
-        <v>231</v>
-      </c>
-      <c r="E5" s="57" t="s">
-        <v>235</v>
-      </c>
-      <c r="F5" s="59" t="s">
-        <v>226</v>
-      </c>
-      <c r="G5" s="58" t="s">
-        <v>230</v>
-      </c>
-      <c r="H5" s="58" t="s">
-        <v>236</v>
-      </c>
-      <c r="I5" s="59" t="s">
-        <v>212</v>
-      </c>
-      <c r="J5" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K5" s="57" t="s">
-        <v>237</v>
+      <c r="N4" s="32"/>
+    </row>
+    <row r="5" spans="1:14" ht="162" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="51"/>
+      <c r="B5" s="54"/>
+      <c r="C5" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>220</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>224</v>
+      </c>
+      <c r="F5" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="J5" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="K5" s="36" t="s">
+        <v>228</v>
       </c>
       <c r="L5" s="23"/>
       <c r="M5" s="25"/>
-      <c r="N5" s="42"/>
-    </row>
-    <row r="6" spans="1:14" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="52"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="60" t="s">
-        <v>238</v>
-      </c>
-      <c r="D6" s="56" t="s">
+      <c r="N5" s="32"/>
+    </row>
+    <row r="6" spans="1:14" ht="204" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="51"/>
+      <c r="B6" s="58" t="s">
+        <v>235</v>
+      </c>
+      <c r="C6" s="59" t="s">
+        <v>236</v>
+      </c>
+      <c r="D6" s="60">
+        <v>6.1</v>
+      </c>
+      <c r="E6" s="61" t="s">
+        <v>237</v>
+      </c>
+      <c r="F6" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="H6" s="63" t="s">
+        <v>239</v>
+      </c>
+      <c r="I6" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="J6" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="64" t="s">
         <v>240</v>
       </c>
-      <c r="E6" s="57"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="62"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="42"/>
-    </row>
-    <row r="7" spans="1:14" ht="282.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="52"/>
-      <c r="B7" s="64"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="59"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="57"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="42"/>
-    </row>
-    <row r="8" spans="1:14" ht="249" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="52"/>
-      <c r="B8" s="54" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="D8" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>204</v>
-      </c>
-      <c r="F8" s="23" t="s">
+      <c r="L6" s="62"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="66"/>
+    </row>
+    <row r="7" spans="1:14" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="51"/>
+      <c r="B7" s="58" t="s">
+        <v>246</v>
+      </c>
+      <c r="C7" s="68" t="s">
+        <v>247</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" s="69" t="s">
+        <v>249</v>
+      </c>
+      <c r="F7" s="55"/>
+      <c r="G7" s="70" t="s">
+        <v>250</v>
+      </c>
+      <c r="H7" s="72" t="s">
+        <v>251</v>
+      </c>
+      <c r="I7" s="73"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="72" t="s">
+        <v>252</v>
+      </c>
+      <c r="L7" s="71"/>
+      <c r="M7" s="71"/>
+      <c r="N7" s="71"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="51"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="51"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="51"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="51"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="51"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="51"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="51"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="51"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="51"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="51"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="51"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="51"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="51"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="51"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="51"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="51"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="51"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="51"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="51"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="51"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="51"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="51"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="51"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="52"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A31"/>
+    <mergeCell ref="B4:B5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB43EE6-FA55-4877-96E9-AE377829827B}">
+  <dimension ref="A1:N31"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:N3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="31.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="0.140625" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="11" max="11" width="27.28515625" customWidth="1"/>
+    <col min="12" max="12" width="25" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="207.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="50"/>
+      <c r="B2" s="33" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>242</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="F2" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H8" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J8" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K8" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L8" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="M8" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N8" s="42"/>
-    </row>
-    <row r="9" spans="1:14" ht="228" x14ac:dyDescent="0.2">
-      <c r="A9" s="52"/>
-      <c r="B9" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>202</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="H9" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="I9" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J9" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K9" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L9" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="M9" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N9" s="42"/>
-    </row>
-    <row r="10" spans="1:14" ht="228" x14ac:dyDescent="0.2">
-      <c r="A10" s="52"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>203</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="H10" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="I10" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J10" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K10" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L10" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="M10" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N10" s="42"/>
-    </row>
-    <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="52"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J11" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K11" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L11" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="M11" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N11" s="42"/>
-    </row>
-    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="52"/>
-      <c r="B12" s="46" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I12" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J12" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K12" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L12" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="M12" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N12" s="42"/>
-    </row>
-    <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="52"/>
-      <c r="B13" s="43"/>
-      <c r="C13" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="E13" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I13" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J13" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K13" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L13" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="M13" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N13" s="42"/>
-    </row>
-    <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="52"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>111</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J14" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K14" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L14" s="23" t="s">
-        <v>114</v>
-      </c>
-      <c r="M14" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N14" s="42"/>
-    </row>
-    <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="52"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>116</v>
-      </c>
-      <c r="E15" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I15" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J15" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K15" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L15" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="M15" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N15" s="42"/>
-    </row>
-    <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="52"/>
-      <c r="B16" s="47" t="s">
-        <v>119</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="D16" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="F16" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I16" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J16" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K16" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L16" s="23" t="s">
-        <v>75</v>
-      </c>
-      <c r="M16" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N16" s="42"/>
-    </row>
-    <row r="17" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="52"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="22" t="s">
-        <v>124</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="E17" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H17" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I17" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J17" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K17" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L17" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="M17" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N17" s="42"/>
-    </row>
-    <row r="18" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="52"/>
-      <c r="B18" s="43"/>
-      <c r="C18" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="E18" s="23" t="s">
-        <v>130</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G18" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H18" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I18" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J18" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K18" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L18" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="M18" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N18" s="42"/>
-    </row>
-    <row r="19" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="52"/>
-      <c r="B19" s="44"/>
-      <c r="C19" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>135</v>
-      </c>
-      <c r="F19" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H19" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I19" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J19" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K19" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L19" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="M19" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N19" s="42"/>
-    </row>
-    <row r="20" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="52"/>
-      <c r="B20" s="48" t="s">
-        <v>137</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="F20" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H20" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I20" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J20" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K20" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L20" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="M20" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N20" s="42"/>
-    </row>
-    <row r="21" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="52"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="E21" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="F21" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G21" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H21" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I21" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J21" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K21" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L21" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="M21" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N21" s="27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="52"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="E22" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="F22" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G22" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H22" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I22" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J22" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K22" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L22" s="23" t="s">
-        <v>150</v>
-      </c>
-      <c r="M22" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N22" s="27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="52"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="E23" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="F23" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G23" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H23" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I23" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J23" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K23" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L23" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="M23" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N23" s="28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="52"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="E24" s="23" t="s">
-        <v>158</v>
-      </c>
-      <c r="F24" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G24" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H24" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I24" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J24" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K24" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L24" s="23" t="s">
-        <v>160</v>
-      </c>
-      <c r="M24" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N24" s="27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="52"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="E25" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="F25" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G25" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H25" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I25" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J25" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K25" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L25" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="M25" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N25" s="27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="52"/>
-      <c r="B26" s="49" t="s">
-        <v>165</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="F26" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G26" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H26" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I26" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J26" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K26" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L26" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="M26" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N26" s="27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="52"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="E27" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="F27" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G27" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H27" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I27" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J27" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K27" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L27" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="M27" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N27" s="27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="52"/>
-      <c r="B28" s="43"/>
-      <c r="C28" s="22" t="s">
-        <v>174</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>175</v>
-      </c>
-      <c r="E28" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="F28" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G28" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H28" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I28" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J28" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K28" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L28" s="23" t="s">
-        <v>178</v>
-      </c>
-      <c r="M28" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N28" s="27" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="52"/>
-      <c r="B29" s="44"/>
-      <c r="C29" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="D29" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="E29" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="F29" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G29" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H29" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I29" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J29" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K29" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L29" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="M29" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N29" s="28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="242.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="52"/>
-      <c r="B30" s="50" t="s">
-        <v>183</v>
-      </c>
-      <c r="C30" s="56" t="s">
-        <v>223</v>
-      </c>
-      <c r="D30" s="56" t="s">
-        <v>225</v>
-      </c>
-      <c r="E30" s="57" t="s">
-        <v>228</v>
-      </c>
-      <c r="F30" s="59" t="s">
-        <v>226</v>
-      </c>
-      <c r="G30" s="58" t="s">
-        <v>230</v>
-      </c>
-      <c r="H30" s="58" t="s">
-        <v>229</v>
-      </c>
-      <c r="I30" s="59" t="s">
-        <v>212</v>
-      </c>
-      <c r="J30" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K30" s="62" t="s">
-        <v>221</v>
-      </c>
-      <c r="L30" s="23"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="42"/>
-    </row>
-    <row r="31" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="G2" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>244</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="J2" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="K2" s="67" t="s">
+        <v>245</v>
+      </c>
+      <c r="L2" s="36"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="32"/>
+    </row>
+    <row r="3" spans="1:14" ht="220.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="51"/>
+      <c r="B3" s="58" t="s">
+        <v>246</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>253</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>242</v>
+      </c>
+      <c r="E3" s="69" t="s">
+        <v>254</v>
+      </c>
+      <c r="F3" s="55"/>
+      <c r="G3" s="70" t="s">
+        <v>250</v>
+      </c>
+      <c r="H3" s="72" t="s">
+        <v>256</v>
+      </c>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="74" t="s">
+        <v>255</v>
+      </c>
+      <c r="L3" s="71"/>
+      <c r="M3" s="71"/>
+      <c r="N3" s="71"/>
+    </row>
+    <row r="4" spans="1:14" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="51"/>
+    </row>
+    <row r="5" spans="1:14" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="51"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="51"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="51"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="51"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="51"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="51"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="51"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="51"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="51"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="51"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="51"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="51"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="51"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="51"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="51"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="51"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="51"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="51"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="51"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="51"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="51"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="51"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="51"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="51"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="51"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="51"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="52"/>
-      <c r="B31" s="43"/>
-      <c r="C31" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="D31" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="E31" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="F31" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G31" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H31" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I31" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J31" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K31" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L31" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="M31" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N31" s="28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="52"/>
-      <c r="B32" s="43"/>
-      <c r="C32" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="D32" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="E32" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="F32" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G32" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H32" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I32" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J32" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K32" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L32" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="M32" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N32" s="28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="53"/>
-      <c r="B33" s="44"/>
-      <c r="C33" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="D33" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="E33" s="23" t="s">
-        <v>199</v>
-      </c>
-      <c r="F33" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="G33" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="H33" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="I33" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="J33" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="K33" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L33" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="M33" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="N33" s="27" t="s">
-        <v>48</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A2:A33"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B20:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="B4:B7"/>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB43EE6-FA55-4877-96E9-AE377829827B}">
-  <dimension ref="A1"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8468A8A-F257-451D-AC30-9124B25FFCDD}">
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D229A3A4-4F9D-42AB-80C8-669754DC12C3}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="24.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.5703125" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" customWidth="1"/>
+    <col min="13" max="13" width="0.140625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>206</v>
-      </c>
+    <row r="1" spans="1:14" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="L1" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" s="34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="174.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="50"/>
+      <c r="B2" s="33" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="35" t="s">
+        <v>258</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>257</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>259</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>260</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="J2" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="K2" s="75" t="s">
+        <v>261</v>
+      </c>
+      <c r="L2" s="36"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="32"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="51"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="51"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="51"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="51"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="51"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="51"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="51"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="51"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="51"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="51"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="51"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="51"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="51"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="51"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="51"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="51"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="51"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="51"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="51"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="51"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="51"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="51"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="51"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="51"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="51"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="51"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="51"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="51"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="52"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A31"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8468A8A-F257-451D-AC30-9124B25FFCDD}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D229A3A4-4F9D-42AB-80C8-669754DC12C3}">
+  <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>207</v>
-      </c>
+    <row r="1" spans="1:13" ht="78.75" x14ac:dyDescent="0.2">
+      <c r="A1" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="M1" s="34" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="179.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="53" t="s">
+        <v>216</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>262</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>263</v>
+      </c>
+      <c r="E2" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>248</v>
+      </c>
+      <c r="G2" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="H2" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="J2" s="75" t="s">
+        <v>265</v>
+      </c>
+      <c r="K2" s="36"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="32"/>
+    </row>
+    <row r="3" spans="1:13" ht="148.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="54"/>
+      <c r="B3" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>262</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>267</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>264</v>
+      </c>
+      <c r="H3" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="J3" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="K3" s="23"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="32"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9142,7 +8900,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -9160,7 +8918,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Login & logout TCs
</commit_message>
<xml_diff>
--- a/5- Testing/Test Cases.xlsx
+++ b/5- Testing/Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Documents\GitHub\Car-Purchasing-App\5- Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1480FA-88A0-4453-AB86-B2AD6C047DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26AD4479-CBB9-4198-A17E-120EFAA153A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="303">
   <si>
     <t>Module</t>
   </si>
@@ -1928,12 +1928,6 @@
     </r>
   </si>
   <si>
-    <t>lo</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
     <t>TC-AddCar-00</t>
   </si>
   <si>
@@ -2185,12 +2179,205 @@
   <si>
     <t>Verify that user sees a pop-up message when there are no cars available for the entered brand name.</t>
   </si>
+  <si>
+    <t>1_logout_user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate that the logout is working from the customer portal 
+</t>
+  </si>
+  <si>
+    <t>Functional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Register page is reachable.
+2. Edge Browser is available.
+3. Availability of test data for "UserID &amp; password".
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+1. Enter '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00FF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>1305892</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>'
+in the user-id Field.
+2. Enter '</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00FF00"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>12345ssss</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>' in the password field.
+3. Press the 'LOGIN' Button.</t>
+    </r>
+  </si>
+  <si>
+    <t>1- user-id : 1305892
+2- password : 12345ssss</t>
+  </si>
+  <si>
+    <t>Fouda</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>the user-id field should accept 
+the user-id and password move to the next 
+page after pressing
+'LOGOUT' successfully</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>PreCondition</t>
+  </si>
+  <si>
+    <t>Priotity</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>Lgn_user_1</t>
+  </si>
+  <si>
+    <t>Validate that the user_id 
+must be filled with valid 
+user_id</t>
+  </si>
+  <si>
+    <t>1. Website login page is reachable.
+2. Browser is available.
+3. The user has to have a valid user_id.
+4. The user has to have a valid password.</t>
+  </si>
+  <si>
+    <t>1. Enter "245668" in the userID field.
+2. Enter "1test&amp;salma" in the Password
+field.
+3. Press Login button.</t>
+  </si>
+  <si>
+    <t>The user should be able to reach
+his data after the login.</t>
+  </si>
+  <si>
+    <t>Lgn_user_2</t>
+  </si>
+  <si>
+    <t>Validate that the user_id 
+field can't be empty.</t>
+  </si>
+  <si>
+    <t>1. Leave the userID field empty.
+2. Enter "1test&amp;salma" in the Password
+field.
+3. Press Login button.</t>
+  </si>
+  <si>
+    <t>An error message should appear
+to that "This field is required".</t>
+  </si>
+  <si>
+    <t>Lgn_user_passwd_3</t>
+  </si>
+  <si>
+    <t>Validate that the password 
+field can't be empty.</t>
+  </si>
+  <si>
+    <t>1. Enter "245668" in the userID field.
+2. Leave the Password
+field empty.
+3. Press Login button.</t>
+  </si>
+  <si>
+    <t>Lgn_user_passwd_4</t>
+  </si>
+  <si>
+    <t>Validate that the password 
+is valid according to the
+user_id.</t>
+  </si>
+  <si>
+    <t>Lgn_Reset_5</t>
+  </si>
+  <si>
+    <t>Validate that after filling the fields and click on reset button
+All data are deleted</t>
+  </si>
+  <si>
+    <t>1. Enter "245668" in the userID field.
+2. Enter "1test&amp;salma" in the Password
+field.
+3. Press reset button.</t>
+  </si>
+  <si>
+    <t>All Fields in the login page 
+are empty again.</t>
+  </si>
+  <si>
+    <t>Lgn_MGR_6</t>
+  </si>
+  <si>
+    <t>Lgn_MGR_7</t>
+  </si>
+  <si>
+    <t>Validate that the mgr given user
+ID and password are 
+working and successfully 
+loged in.</t>
+  </si>
+  <si>
+    <t>1. Enter "mngr479920" in the userID field.
+2. Enter "yvAtyja" in the Password
+field.
+3. Press Login button.</t>
+  </si>
+  <si>
+    <t>The mgr should be able to 
+login successfully in the home page.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2322,8 +2509,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00FF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="28">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2486,8 +2699,26 @@
         <bgColor rgb="FFFF00FF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF073763"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9DAF8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -2599,11 +2830,146 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF434343"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF434343"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF434343"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF434343"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF434343"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF434343"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2722,6 +3088,64 @@
     <xf numFmtId="0" fontId="16" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2759,65 +3183,40 @@
     <xf numFmtId="0" fontId="13" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6644,7 +7043,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="140.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="60" t="s">
         <v>57</v>
       </c>
       <c r="B2" s="21" t="s">
@@ -6691,8 +7090,8 @@
       </c>
     </row>
     <row r="3" spans="1:15" ht="147" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="41"/>
-      <c r="B3" s="43" t="s">
+      <c r="A3" s="61"/>
+      <c r="B3" s="63" t="s">
         <v>69</v>
       </c>
       <c r="C3" s="22" t="s">
@@ -6736,8 +7135,8 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="138.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="41"/>
-      <c r="B4" s="41"/>
+      <c r="A4" s="61"/>
+      <c r="B4" s="61"/>
       <c r="C4" s="22" t="s">
         <v>76</v>
       </c>
@@ -6779,8 +7178,8 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="41"/>
-      <c r="B5" s="41"/>
+      <c r="A5" s="61"/>
+      <c r="B5" s="61"/>
       <c r="C5" s="22" t="s">
         <v>80</v>
       </c>
@@ -6822,8 +7221,8 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="145.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="41"/>
-      <c r="B6" s="42"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="62"/>
       <c r="C6" s="22" t="s">
         <v>84</v>
       </c>
@@ -6865,8 +7264,8 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="138" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="41"/>
-      <c r="B7" s="44" t="s">
+      <c r="A7" s="61"/>
+      <c r="B7" s="64" t="s">
         <v>89</v>
       </c>
       <c r="C7" s="22" t="s">
@@ -6910,8 +7309,8 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="145.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
+      <c r="A8" s="61"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="22" t="s">
         <v>94</v>
       </c>
@@ -6953,8 +7352,8 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="145.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="41"/>
-      <c r="B9" s="42"/>
+      <c r="A9" s="61"/>
+      <c r="B9" s="62"/>
       <c r="C9" s="22" t="s">
         <v>97</v>
       </c>
@@ -6996,8 +7395,8 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="41"/>
-      <c r="B10" s="45" t="s">
+      <c r="A10" s="61"/>
+      <c r="B10" s="65" t="s">
         <v>101</v>
       </c>
       <c r="C10" s="22" t="s">
@@ -7041,8 +7440,8 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41"/>
+      <c r="A11" s="61"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="22" t="s">
         <v>106</v>
       </c>
@@ -7084,8 +7483,8 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
+      <c r="A12" s="61"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="22" t="s">
         <v>110</v>
       </c>
@@ -7127,8 +7526,8 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="41"/>
-      <c r="B13" s="42"/>
+      <c r="A13" s="61"/>
+      <c r="B13" s="62"/>
       <c r="C13" s="22" t="s">
         <v>115</v>
       </c>
@@ -7170,8 +7569,8 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A14" s="41"/>
-      <c r="B14" s="46" t="s">
+      <c r="A14" s="61"/>
+      <c r="B14" s="66" t="s">
         <v>119</v>
       </c>
       <c r="C14" s="22" t="s">
@@ -7215,8 +7614,8 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="41"/>
-      <c r="B15" s="41"/>
+      <c r="A15" s="61"/>
+      <c r="B15" s="61"/>
       <c r="C15" s="22" t="s">
         <v>124</v>
       </c>
@@ -7258,8 +7657,8 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="41"/>
-      <c r="B16" s="41"/>
+      <c r="A16" s="61"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="22" t="s">
         <v>128</v>
       </c>
@@ -7301,8 +7700,8 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="41"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="61"/>
+      <c r="B17" s="62"/>
       <c r="C17" s="22" t="s">
         <v>133</v>
       </c>
@@ -7344,8 +7743,8 @@
       </c>
     </row>
     <row r="18" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="41"/>
-      <c r="B18" s="47" t="s">
+      <c r="A18" s="61"/>
+      <c r="B18" s="67" t="s">
         <v>137</v>
       </c>
       <c r="C18" s="22" t="s">
@@ -7389,8 +7788,8 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="61"/>
+      <c r="B19" s="61"/>
       <c r="C19" s="22" t="s">
         <v>142</v>
       </c>
@@ -7432,8 +7831,8 @@
       </c>
     </row>
     <row r="20" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="41"/>
-      <c r="B20" s="41"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="22" t="s">
         <v>146</v>
       </c>
@@ -7475,8 +7874,8 @@
       </c>
     </row>
     <row r="21" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="41"/>
-      <c r="B21" s="41"/>
+      <c r="A21" s="61"/>
+      <c r="B21" s="61"/>
       <c r="C21" s="22" t="s">
         <v>151</v>
       </c>
@@ -7518,8 +7917,8 @@
       </c>
     </row>
     <row r="22" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="41"/>
-      <c r="B22" s="41"/>
+      <c r="A22" s="61"/>
+      <c r="B22" s="61"/>
       <c r="C22" s="22" t="s">
         <v>156</v>
       </c>
@@ -7561,8 +7960,8 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="41"/>
-      <c r="B23" s="42"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="62"/>
       <c r="C23" s="22" t="s">
         <v>161</v>
       </c>
@@ -7604,8 +8003,8 @@
       </c>
     </row>
     <row r="24" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="41"/>
-      <c r="B24" s="48" t="s">
+      <c r="A24" s="61"/>
+      <c r="B24" s="68" t="s">
         <v>165</v>
       </c>
       <c r="C24" s="22" t="s">
@@ -7649,8 +8048,8 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="41"/>
-      <c r="B25" s="41"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="61"/>
       <c r="C25" s="22" t="s">
         <v>170</v>
       </c>
@@ -7692,8 +8091,8 @@
       </c>
     </row>
     <row r="26" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="41"/>
-      <c r="B26" s="41"/>
+      <c r="A26" s="61"/>
+      <c r="B26" s="61"/>
       <c r="C26" s="22" t="s">
         <v>174</v>
       </c>
@@ -7735,8 +8134,8 @@
       </c>
     </row>
     <row r="27" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="41"/>
-      <c r="B27" s="42"/>
+      <c r="A27" s="61"/>
+      <c r="B27" s="62"/>
       <c r="C27" s="22" t="s">
         <v>179</v>
       </c>
@@ -7778,8 +8177,8 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="41"/>
-      <c r="B28" s="49" t="s">
+      <c r="A28" s="61"/>
+      <c r="B28" s="69" t="s">
         <v>183</v>
       </c>
       <c r="C28" s="22" t="s">
@@ -7823,8 +8222,8 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="41"/>
-      <c r="B29" s="41"/>
+      <c r="A29" s="61"/>
+      <c r="B29" s="61"/>
       <c r="C29" s="22" t="s">
         <v>189</v>
       </c>
@@ -7866,8 +8265,8 @@
       </c>
     </row>
     <row r="30" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="41"/>
-      <c r="B30" s="41"/>
+      <c r="A30" s="61"/>
+      <c r="B30" s="61"/>
       <c r="C30" s="22" t="s">
         <v>193</v>
       </c>
@@ -7909,8 +8308,8 @@
       </c>
     </row>
     <row r="31" spans="1:15" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="42"/>
-      <c r="B31" s="42"/>
+      <c r="A31" s="62"/>
+      <c r="B31" s="62"/>
       <c r="C31" s="22" t="s">
         <v>197</v>
       </c>
@@ -8001,7 +8400,7 @@
         <v>49</v>
       </c>
       <c r="D1" s="39" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E1" s="34" t="s">
         <v>38</v>
@@ -8035,284 +8434,284 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="207" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="50"/>
+      <c r="A2" s="70"/>
       <c r="B2" s="33" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D2" s="38" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E2" s="36" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F2" s="23" t="s">
         <v>47</v>
       </c>
       <c r="G2" s="36" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H2" s="36" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I2" s="37" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J2" s="37" t="s">
-        <v>210</v>
-      </c>
-      <c r="K2" s="56" t="s">
-        <v>226</v>
+        <v>208</v>
+      </c>
+      <c r="K2" s="41" t="s">
+        <v>224</v>
       </c>
       <c r="L2" s="36"/>
       <c r="M2" s="31"/>
       <c r="N2" s="32"/>
     </row>
     <row r="3" spans="1:14" ht="175.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="51"/>
+      <c r="A3" s="71"/>
       <c r="B3" s="33" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>219</v>
+      </c>
+      <c r="D3" s="35" t="s">
         <v>213</v>
       </c>
-      <c r="C3" s="38" t="s">
-        <v>221</v>
-      </c>
-      <c r="D3" s="35" t="s">
-        <v>215</v>
-      </c>
       <c r="E3" s="36" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G3" s="36" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H3" s="36" t="s">
+        <v>230</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="J3" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="K3" s="42" t="s">
         <v>232</v>
-      </c>
-      <c r="I3" s="37" t="s">
-        <v>209</v>
-      </c>
-      <c r="J3" s="37" t="s">
-        <v>210</v>
-      </c>
-      <c r="K3" s="57" t="s">
-        <v>234</v>
       </c>
       <c r="L3" s="30"/>
       <c r="M3" s="31"/>
       <c r="N3" s="32"/>
     </row>
     <row r="4" spans="1:14" ht="142.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="51"/>
-      <c r="B4" s="53" t="s">
+      <c r="A4" s="71"/>
+      <c r="B4" s="73" t="s">
+        <v>214</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>220</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>215</v>
+      </c>
+      <c r="E4" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="F4" s="37" t="s">
         <v>216</v>
       </c>
-      <c r="C4" s="38" t="s">
-        <v>222</v>
-      </c>
-      <c r="D4" s="35" t="s">
+      <c r="G4" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="H4" s="36" t="s">
+        <v>228</v>
+      </c>
+      <c r="I4" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="J4" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="K4" s="42" t="s">
         <v>229</v>
-      </c>
-      <c r="F4" s="37" t="s">
-        <v>218</v>
-      </c>
-      <c r="G4" s="36" t="s">
-        <v>219</v>
-      </c>
-      <c r="H4" s="36" t="s">
-        <v>230</v>
-      </c>
-      <c r="I4" s="37" t="s">
-        <v>209</v>
-      </c>
-      <c r="J4" s="37" t="s">
-        <v>210</v>
-      </c>
-      <c r="K4" s="57" t="s">
-        <v>231</v>
       </c>
       <c r="L4" s="23"/>
       <c r="M4" s="25"/>
       <c r="N4" s="32"/>
     </row>
     <row r="5" spans="1:14" ht="162" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="51"/>
-      <c r="B5" s="54"/>
+      <c r="A5" s="71"/>
+      <c r="B5" s="74"/>
       <c r="C5" s="38" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E5" s="36" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G5" s="36" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H5" s="36" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I5" s="37" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="K5" s="36" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="L5" s="23"/>
       <c r="M5" s="25"/>
       <c r="N5" s="32"/>
     </row>
     <row r="6" spans="1:14" ht="204" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="51"/>
-      <c r="B6" s="58" t="s">
+      <c r="A6" s="71"/>
+      <c r="B6" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>234</v>
+      </c>
+      <c r="D6" s="45">
+        <v>6.1</v>
+      </c>
+      <c r="E6" s="46" t="s">
         <v>235</v>
       </c>
-      <c r="C6" s="59" t="s">
-        <v>236</v>
-      </c>
-      <c r="D6" s="60">
-        <v>6.1</v>
-      </c>
-      <c r="E6" s="61" t="s">
+      <c r="F6" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="H6" s="48" t="s">
         <v>237</v>
       </c>
-      <c r="F6" s="62" t="s">
-        <v>47</v>
-      </c>
-      <c r="G6" s="36" t="s">
-        <v>219</v>
-      </c>
-      <c r="H6" s="63" t="s">
-        <v>239</v>
-      </c>
-      <c r="I6" s="62" t="s">
+      <c r="I6" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="J6" s="62" t="s">
+      <c r="J6" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="K6" s="64" t="s">
-        <v>240</v>
-      </c>
-      <c r="L6" s="62"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="66"/>
+      <c r="K6" s="49" t="s">
+        <v>238</v>
+      </c>
+      <c r="L6" s="47"/>
+      <c r="M6" s="50"/>
+      <c r="N6" s="51"/>
     </row>
     <row r="7" spans="1:14" ht="91.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="51"/>
-      <c r="B7" s="58" t="s">
-        <v>246</v>
-      </c>
-      <c r="C7" s="68" t="s">
+      <c r="A7" s="71"/>
+      <c r="B7" s="43" t="s">
+        <v>244</v>
+      </c>
+      <c r="C7" s="53" t="s">
+        <v>245</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>210</v>
+      </c>
+      <c r="E7" s="54" t="s">
         <v>247</v>
       </c>
-      <c r="D7" s="38" t="s">
-        <v>212</v>
-      </c>
-      <c r="E7" s="69" t="s">
+      <c r="F7" s="40"/>
+      <c r="G7" s="55" t="s">
+        <v>248</v>
+      </c>
+      <c r="H7" s="57" t="s">
         <v>249</v>
       </c>
-      <c r="F7" s="55"/>
-      <c r="G7" s="70" t="s">
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="57" t="s">
         <v>250</v>
       </c>
-      <c r="H7" s="72" t="s">
-        <v>251</v>
-      </c>
-      <c r="I7" s="73"/>
-      <c r="J7" s="73"/>
-      <c r="K7" s="72" t="s">
-        <v>252</v>
-      </c>
-      <c r="L7" s="71"/>
-      <c r="M7" s="71"/>
-      <c r="N7" s="71"/>
+      <c r="L7" s="56"/>
+      <c r="M7" s="56"/>
+      <c r="N7" s="56"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="51"/>
+      <c r="A8" s="71"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="51"/>
+      <c r="A9" s="71"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="51"/>
+      <c r="A10" s="71"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="51"/>
+      <c r="A11" s="71"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="51"/>
+      <c r="A12" s="71"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="51"/>
+      <c r="A13" s="71"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="51"/>
+      <c r="A14" s="71"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="51"/>
+      <c r="A15" s="71"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="51"/>
+      <c r="A16" s="71"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="51"/>
+      <c r="A17" s="71"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="51"/>
+      <c r="A18" s="71"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="51"/>
+      <c r="A19" s="71"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="51"/>
+      <c r="A20" s="71"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="51"/>
+      <c r="A21" s="71"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="51"/>
+      <c r="A22" s="71"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="51"/>
+      <c r="A23" s="71"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="51"/>
+      <c r="A24" s="71"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="51"/>
+      <c r="A25" s="71"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="51"/>
+      <c r="A26" s="71"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="51"/>
+      <c r="A27" s="71"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="51"/>
+      <c r="A28" s="71"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="51"/>
+      <c r="A29" s="71"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="51"/>
+      <c r="A30" s="71"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="52"/>
+      <c r="A31" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8359,7 +8758,7 @@
         <v>49</v>
       </c>
       <c r="D1" s="39" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E1" s="34" t="s">
         <v>38</v>
@@ -8393,154 +8792,154 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="207.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="50"/>
+      <c r="A2" s="70"/>
       <c r="B2" s="33" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C2" s="35" t="s">
+        <v>239</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="E2" s="36" t="s">
         <v>241</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>242</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>243</v>
       </c>
       <c r="F2" s="23" t="s">
         <v>47</v>
       </c>
       <c r="G2" s="36" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="H2" s="36" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="I2" s="37" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J2" s="37" t="s">
-        <v>210</v>
-      </c>
-      <c r="K2" s="67" t="s">
-        <v>245</v>
+        <v>208</v>
+      </c>
+      <c r="K2" s="52" t="s">
+        <v>243</v>
       </c>
       <c r="L2" s="36"/>
       <c r="M2" s="31"/>
       <c r="N2" s="32"/>
     </row>
     <row r="3" spans="1:14" ht="220.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="51"/>
-      <c r="B3" s="58" t="s">
-        <v>246</v>
-      </c>
-      <c r="C3" s="68" t="s">
+      <c r="A3" s="71"/>
+      <c r="B3" s="43" t="s">
+        <v>244</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>251</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="E3" s="54" t="s">
+        <v>252</v>
+      </c>
+      <c r="F3" s="40"/>
+      <c r="G3" s="55" t="s">
+        <v>248</v>
+      </c>
+      <c r="H3" s="57" t="s">
+        <v>254</v>
+      </c>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="59" t="s">
         <v>253</v>
       </c>
-      <c r="D3" s="38" t="s">
-        <v>242</v>
-      </c>
-      <c r="E3" s="69" t="s">
-        <v>254</v>
-      </c>
-      <c r="F3" s="55"/>
-      <c r="G3" s="70" t="s">
-        <v>250</v>
-      </c>
-      <c r="H3" s="72" t="s">
-        <v>256</v>
-      </c>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="74" t="s">
-        <v>255</v>
-      </c>
-      <c r="L3" s="71"/>
-      <c r="M3" s="71"/>
-      <c r="N3" s="71"/>
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
     </row>
     <row r="4" spans="1:14" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="51"/>
+      <c r="A4" s="71"/>
     </row>
     <row r="5" spans="1:14" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="51"/>
+      <c r="A5" s="71"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="51"/>
+      <c r="A6" s="71"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="51"/>
+      <c r="A7" s="71"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="51"/>
+      <c r="A8" s="71"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="51"/>
+      <c r="A9" s="71"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="51"/>
+      <c r="A10" s="71"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="51"/>
+      <c r="A11" s="71"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="51"/>
+      <c r="A12" s="71"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="51"/>
+      <c r="A13" s="71"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="51"/>
+      <c r="A14" s="71"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="51"/>
+      <c r="A15" s="71"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="51"/>
+      <c r="A16" s="71"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="51"/>
+      <c r="A17" s="71"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="51"/>
+      <c r="A18" s="71"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="51"/>
+      <c r="A19" s="71"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="51"/>
+      <c r="A20" s="71"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="51"/>
+      <c r="A21" s="71"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="51"/>
+      <c r="A22" s="71"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="51"/>
+      <c r="A23" s="71"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="51"/>
+      <c r="A24" s="71"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="51"/>
+      <c r="A25" s="71"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="51"/>
+      <c r="A26" s="71"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="51"/>
+      <c r="A27" s="71"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="51"/>
+      <c r="A28" s="71"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="51"/>
+      <c r="A29" s="71"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="51"/>
+      <c r="A30" s="71"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="52"/>
+      <c r="A31" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8585,7 +8984,7 @@
         <v>49</v>
       </c>
       <c r="D1" s="39" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="E1" s="34" t="s">
         <v>38</v>
@@ -8619,127 +9018,127 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="174.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="50"/>
+      <c r="A2" s="70"/>
       <c r="B2" s="33" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C2" s="35" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D2" s="38" t="s">
+        <v>255</v>
+      </c>
+      <c r="E2" s="36" t="s">
         <v>257</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>259</v>
       </c>
       <c r="F2" s="23" t="s">
         <v>47</v>
       </c>
       <c r="G2" s="36" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H2" s="36" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I2" s="37" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J2" s="37" t="s">
-        <v>210</v>
-      </c>
-      <c r="K2" s="75" t="s">
-        <v>261</v>
+        <v>208</v>
+      </c>
+      <c r="K2" s="54" t="s">
+        <v>259</v>
       </c>
       <c r="L2" s="36"/>
       <c r="M2" s="31"/>
       <c r="N2" s="32"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="51"/>
+      <c r="A3" s="71"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="51"/>
+      <c r="A4" s="71"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" s="51"/>
+      <c r="A5" s="71"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="51"/>
+      <c r="A6" s="71"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" s="51"/>
+      <c r="A7" s="71"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A8" s="51"/>
+      <c r="A8" s="71"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A9" s="51"/>
+      <c r="A9" s="71"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A10" s="51"/>
+      <c r="A10" s="71"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" s="51"/>
+      <c r="A11" s="71"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A12" s="51"/>
+      <c r="A12" s="71"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A13" s="51"/>
+      <c r="A13" s="71"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A14" s="51"/>
+      <c r="A14" s="71"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A15" s="51"/>
+      <c r="A15" s="71"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="51"/>
+      <c r="A16" s="71"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="51"/>
+      <c r="A17" s="71"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="51"/>
+      <c r="A18" s="71"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="51"/>
+      <c r="A19" s="71"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="51"/>
+      <c r="A20" s="71"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="51"/>
+      <c r="A21" s="71"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="51"/>
+      <c r="A22" s="71"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="51"/>
+      <c r="A23" s="71"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="51"/>
+      <c r="A24" s="71"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="51"/>
+      <c r="A25" s="71"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="51"/>
+      <c r="A26" s="71"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="51"/>
+      <c r="A27" s="71"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="51"/>
+      <c r="A28" s="71"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="51"/>
+      <c r="A29" s="71"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="51"/>
+      <c r="A30" s="71"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="52"/>
+      <c r="A31" s="72"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8753,7 +9152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D229A3A4-4F9D-42AB-80C8-669754DC12C3}">
   <dimension ref="A1:M3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
@@ -8773,7 +9172,7 @@
     <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="78.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A1" s="34" t="s">
         <v>54</v>
       </c>
@@ -8781,7 +9180,7 @@
         <v>49</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D1" s="34" t="s">
         <v>38</v>
@@ -8815,68 +9214,68 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="179.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="53" t="s">
-        <v>216</v>
+      <c r="A2" s="73" t="s">
+        <v>214</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E2" s="23" t="s">
         <v>47</v>
       </c>
       <c r="F2" s="36" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G2" s="36" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="H2" s="37" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I2" s="37" t="s">
-        <v>210</v>
-      </c>
-      <c r="J2" s="75" t="s">
-        <v>265</v>
+        <v>208</v>
+      </c>
+      <c r="J2" s="54" t="s">
+        <v>263</v>
       </c>
       <c r="K2" s="36"/>
       <c r="L2" s="25"/>
       <c r="M2" s="32"/>
     </row>
     <row r="3" spans="1:13" ht="148.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="54"/>
+      <c r="A3" s="74"/>
       <c r="B3" s="38" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C3" s="38" t="s">
+        <v>260</v>
+      </c>
+      <c r="D3" s="36" t="s">
+        <v>265</v>
+      </c>
+      <c r="E3" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>217</v>
+      </c>
+      <c r="G3" s="36" t="s">
         <v>262</v>
       </c>
-      <c r="D3" s="36" t="s">
-        <v>267</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>218</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>219</v>
-      </c>
-      <c r="G3" s="36" t="s">
-        <v>264</v>
-      </c>
       <c r="H3" s="37" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I3" s="37" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J3" s="36" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K3" s="23"/>
       <c r="L3" s="25"/>
@@ -8892,16 +9291,267 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E3E3723-9A66-41B9-B3EE-9ACDC170719F}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>206</v>
-      </c>
+    <row r="1" spans="1:12" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="80" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="81" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="81" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="81" t="s">
+        <v>276</v>
+      </c>
+      <c r="E1" s="81" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="81" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="81" t="s">
+        <v>277</v>
+      </c>
+      <c r="H1" s="81" t="s">
+        <v>278</v>
+      </c>
+      <c r="I1" s="81" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="81" t="s">
+        <v>279</v>
+      </c>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+    </row>
+    <row r="2" spans="1:12" ht="204.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="82" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2" s="83" t="s">
+        <v>281</v>
+      </c>
+      <c r="C2" s="83" t="s">
+        <v>268</v>
+      </c>
+      <c r="D2" s="83" t="s">
+        <v>282</v>
+      </c>
+      <c r="E2" s="83" t="s">
+        <v>283</v>
+      </c>
+      <c r="F2" s="83" t="s">
+        <v>272</v>
+      </c>
+      <c r="G2" s="83" t="s">
+        <v>208</v>
+      </c>
+      <c r="H2" s="83" t="s">
+        <v>284</v>
+      </c>
+      <c r="I2" s="84"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+    </row>
+    <row r="3" spans="1:12" ht="234" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="82" t="s">
+        <v>285</v>
+      </c>
+      <c r="B3" s="83" t="s">
+        <v>286</v>
+      </c>
+      <c r="C3" s="83" t="s">
+        <v>268</v>
+      </c>
+      <c r="D3" s="83" t="s">
+        <v>282</v>
+      </c>
+      <c r="E3" s="83" t="s">
+        <v>287</v>
+      </c>
+      <c r="F3" s="83" t="s">
+        <v>272</v>
+      </c>
+      <c r="G3" s="83" t="s">
+        <v>208</v>
+      </c>
+      <c r="H3" s="83" t="s">
+        <v>288</v>
+      </c>
+      <c r="I3" s="84"/>
+      <c r="J3" s="83"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+    </row>
+    <row r="4" spans="1:12" ht="239.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="82" t="s">
+        <v>289</v>
+      </c>
+      <c r="B4" s="83" t="s">
+        <v>290</v>
+      </c>
+      <c r="C4" s="83" t="s">
+        <v>268</v>
+      </c>
+      <c r="D4" s="83" t="s">
+        <v>282</v>
+      </c>
+      <c r="E4" s="83" t="s">
+        <v>291</v>
+      </c>
+      <c r="F4" s="83" t="s">
+        <v>272</v>
+      </c>
+      <c r="G4" s="83" t="s">
+        <v>208</v>
+      </c>
+      <c r="H4" s="83" t="s">
+        <v>288</v>
+      </c>
+      <c r="I4" s="84"/>
+      <c r="J4" s="83"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="75"/>
+    </row>
+    <row r="5" spans="1:12" ht="221.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="82" t="s">
+        <v>292</v>
+      </c>
+      <c r="B5" s="83" t="s">
+        <v>293</v>
+      </c>
+      <c r="C5" s="83" t="s">
+        <v>268</v>
+      </c>
+      <c r="D5" s="83" t="s">
+        <v>282</v>
+      </c>
+      <c r="E5" s="83" t="s">
+        <v>283</v>
+      </c>
+      <c r="F5" s="83" t="s">
+        <v>272</v>
+      </c>
+      <c r="G5" s="83" t="s">
+        <v>208</v>
+      </c>
+      <c r="H5" s="83" t="s">
+        <v>284</v>
+      </c>
+      <c r="I5" s="84"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="75"/>
+      <c r="L5" s="75"/>
+    </row>
+    <row r="6" spans="1:12" ht="233.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="82" t="s">
+        <v>294</v>
+      </c>
+      <c r="B6" s="85" t="s">
+        <v>295</v>
+      </c>
+      <c r="C6" s="85" t="s">
+        <v>268</v>
+      </c>
+      <c r="D6" s="83" t="s">
+        <v>282</v>
+      </c>
+      <c r="E6" s="83" t="s">
+        <v>296</v>
+      </c>
+      <c r="F6" s="83" t="s">
+        <v>272</v>
+      </c>
+      <c r="G6" s="83" t="s">
+        <v>208</v>
+      </c>
+      <c r="H6" s="85" t="s">
+        <v>297</v>
+      </c>
+      <c r="I6" s="84"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="75"/>
+    </row>
+    <row r="7" spans="1:12" ht="207.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="82" t="s">
+        <v>298</v>
+      </c>
+      <c r="B7" s="83" t="s">
+        <v>286</v>
+      </c>
+      <c r="C7" s="83" t="s">
+        <v>268</v>
+      </c>
+      <c r="D7" s="83" t="s">
+        <v>282</v>
+      </c>
+      <c r="E7" s="83" t="s">
+        <v>287</v>
+      </c>
+      <c r="F7" s="83" t="s">
+        <v>272</v>
+      </c>
+      <c r="G7" s="83" t="s">
+        <v>208</v>
+      </c>
+      <c r="H7" s="83" t="s">
+        <v>288</v>
+      </c>
+      <c r="I7" s="84"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="75"/>
+      <c r="L7" s="75"/>
+    </row>
+    <row r="8" spans="1:12" ht="249.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="82" t="s">
+        <v>299</v>
+      </c>
+      <c r="B8" s="86" t="s">
+        <v>300</v>
+      </c>
+      <c r="C8" s="83" t="s">
+        <v>268</v>
+      </c>
+      <c r="D8" s="83" t="s">
+        <v>282</v>
+      </c>
+      <c r="E8" s="83" t="s">
+        <v>301</v>
+      </c>
+      <c r="F8" s="83" t="s">
+        <v>272</v>
+      </c>
+      <c r="G8" s="83" t="s">
+        <v>208</v>
+      </c>
+      <c r="H8" s="86" t="s">
+        <v>302</v>
+      </c>
+      <c r="I8" s="84"/>
+      <c r="J8" s="83"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="75"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8910,19 +9560,91 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ADD30B2-DD71-45BD-B5D3-ECBDD8B20B47}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>207</v>
-      </c>
+    <row r="1" spans="1:11" ht="32.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="78" t="s">
+        <v>275</v>
+      </c>
+      <c r="B1" s="79" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="79" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="79" t="s">
+        <v>276</v>
+      </c>
+      <c r="E1" s="79" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="79" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="79" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="79" t="s">
+        <v>277</v>
+      </c>
+      <c r="I1" s="79" t="s">
+        <v>278</v>
+      </c>
+      <c r="J1" s="79" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="75"/>
+    </row>
+    <row r="2" spans="1:11" ht="210" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="76" t="s">
+        <v>266</v>
+      </c>
+      <c r="B2" s="77" t="s">
+        <v>267</v>
+      </c>
+      <c r="C2" s="77" t="s">
+        <v>268</v>
+      </c>
+      <c r="D2" s="77" t="s">
+        <v>269</v>
+      </c>
+      <c r="E2" s="77" t="s">
+        <v>270</v>
+      </c>
+      <c r="F2" s="77" t="s">
+        <v>271</v>
+      </c>
+      <c r="G2" s="77" t="s">
+        <v>272</v>
+      </c>
+      <c r="H2" s="77" t="s">
+        <v>273</v>
+      </c>
+      <c r="I2" s="77" t="s">
+        <v>274</v>
+      </c>
+      <c r="J2" s="77"/>
+      <c r="K2" s="75"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
edit search feature TCs
</commit_message>
<xml_diff>
--- a/5- Testing/Test Cases.xlsx
+++ b/5- Testing/Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Documents\GitHub\Car-Purchasing-App\5- Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CED83D6-7B93-4F54-BFAA-50BD81DA65F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67734037-DA76-4EB6-A748-4A219F68110F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="146">
   <si>
     <t>Module</t>
   </si>
@@ -368,9 +368,6 @@
   </si>
   <si>
     <t>The system should display a list of cars that match the toyota brand.</t>
-  </si>
-  <si>
-    <t>TC-SearchBrand-00</t>
   </si>
   <si>
     <t>Verify that user sees a pop-up message when there are no cars available for the entered brand name.</t>
@@ -567,6 +564,89 @@
   <si>
     <t>The mgr should be able to 
 login successfully in the home page.</t>
+  </si>
+  <si>
+    <t>Brand Field(User)</t>
+  </si>
+  <si>
+    <t>TC-SearchBrand
+-User-00</t>
+  </si>
+  <si>
+    <t>TC-SearchBrand
+-User-01</t>
+  </si>
+  <si>
+    <t>REQ-5.1</t>
+  </si>
+  <si>
+    <t>1. Click on the search bar.
+2. Enter "ferrari " in the search bar.
+3. Click on the search button.
+.</t>
+  </si>
+  <si>
+    <t>A pop up message should appear "please try another brand or range of price"</t>
+  </si>
+  <si>
+    <t>Price Field (User)</t>
+  </si>
+  <si>
+    <t>TC-SearchPrice
+-User-02</t>
+  </si>
+  <si>
+    <t>Verify if the user can search for cars by  price.</t>
+  </si>
+  <si>
+    <t>1. Click on the search bar.
+2. Enter "500,000 " in the search bar.
+3. Click on the search button.
+.</t>
+  </si>
+  <si>
+    <t>The system should display a list of cars that match the price the user entered.</t>
+  </si>
+  <si>
+    <t>TC-SearchPrice
+-User-03</t>
+  </si>
+  <si>
+    <t>Verify that user sees a pop-up message when there are no cars available for the entered price.</t>
+  </si>
+  <si>
+    <t>Brand Field(Admin)</t>
+  </si>
+  <si>
+    <t>TC-SearchBrand
+-Admin-04</t>
+  </si>
+  <si>
+    <t>Verify if the admin can search for cars by  brand name.</t>
+  </si>
+  <si>
+    <t>TC-SearchBrand
+-Admin-05</t>
+  </si>
+  <si>
+    <t>Verify that admin sees a pop-up message when there are no cars available for the entered brand name.</t>
+  </si>
+  <si>
+    <t>Price Field (Admin)</t>
+  </si>
+  <si>
+    <t>TC-SearchPrice
+-Admin-06</t>
+  </si>
+  <si>
+    <t>Verify if the admin can search for cars by  price.</t>
+  </si>
+  <si>
+    <t>TC-SearchPrice
+-Admin-07</t>
+  </si>
+  <si>
+    <t>Verify that admin sees a pop-up message when there are no cars available for the entered price.</t>
   </si>
 </sst>
 </file>
@@ -1501,7 +1581,7 @@
   </sheetPr>
   <dimension ref="A1:AE996"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:K14"/>
     </sheetView>
   </sheetViews>
@@ -1766,7 +1846,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="18" t="e">
-        <f t="shared" ref="K3:K15" si="1">(G15/F15)*100</f>
+        <f t="shared" ref="K15" si="1">(G15/F15)*100</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -5505,10 +5585,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D229A3A4-4F9D-42AB-80C8-669754DC12C3}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5570,10 +5650,10 @@
     </row>
     <row r="2" spans="1:13" ht="179.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="67" t="s">
-        <v>35</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>85</v>
+        <v>123</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>124</v>
       </c>
       <c r="C2" s="30" t="s">
         <v>81</v>
@@ -5606,22 +5686,22 @@
     <row r="3" spans="1:13" ht="148.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="68"/>
       <c r="B3" s="30" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>81</v>
+        <v>126</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>37</v>
+        <v>85</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>21</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>83</v>
+        <v>127</v>
       </c>
       <c r="H3" s="29" t="s">
         <v>28</v>
@@ -5629,16 +5709,219 @@
       <c r="I3" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="K3" s="20"/>
+      <c r="J3" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="K3" s="28"/>
       <c r="L3" s="21"/>
       <c r="M3" s="24"/>
     </row>
+    <row r="4" spans="1:13" ht="114" x14ac:dyDescent="0.2">
+      <c r="A4" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="K4" s="28"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="24"/>
+    </row>
+    <row r="5" spans="1:13" ht="114" x14ac:dyDescent="0.2">
+      <c r="A5" s="68"/>
+      <c r="B5" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H5" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="K5" s="20"/>
+    </row>
+    <row r="6" spans="1:13" ht="114" x14ac:dyDescent="0.2">
+      <c r="A6" s="67" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="H6" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="K6" s="28"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="24"/>
+    </row>
+    <row r="7" spans="1:13" ht="114" x14ac:dyDescent="0.2">
+      <c r="A7" s="68"/>
+      <c r="B7" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="H7" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="K7" s="28"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="24"/>
+    </row>
+    <row r="8" spans="1:13" ht="114" x14ac:dyDescent="0.2">
+      <c r="A8" s="67" t="s">
+        <v>141</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="46" t="s">
+        <v>133</v>
+      </c>
+      <c r="K8" s="28"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="24"/>
+    </row>
+    <row r="9" spans="1:13" ht="114" x14ac:dyDescent="0.2">
+      <c r="A9" s="68"/>
+      <c r="B9" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H9" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="J9" s="46" t="s">
+        <v>128</v>
+      </c>
+      <c r="K9" s="20"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5675,7 +5958,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E1" s="58" t="s">
         <v>15</v>
@@ -5684,44 +5967,44 @@
         <v>17</v>
       </c>
       <c r="G1" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="58" t="s">
         <v>98</v>
-      </c>
-      <c r="H1" s="58" t="s">
-        <v>99</v>
       </c>
       <c r="I1" s="58" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="58" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K1" s="52"/>
       <c r="L1" s="52"/>
     </row>
     <row r="2" spans="1:12" ht="204.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="60" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="60" t="s">
+      <c r="C2" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="60" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="60" t="s">
+      <c r="E2" s="60" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="60" t="s">
-        <v>104</v>
-      </c>
       <c r="F2" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G2" s="60" t="s">
         <v>29</v>
       </c>
       <c r="H2" s="60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I2" s="61"/>
       <c r="J2" s="60"/>
@@ -5730,28 +6013,28 @@
     </row>
     <row r="3" spans="1:12" ht="234" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="C3" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" s="60" t="s">
-        <v>108</v>
-      </c>
       <c r="F3" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G3" s="60" t="s">
         <v>29</v>
       </c>
       <c r="H3" s="60" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I3" s="61"/>
       <c r="J3" s="60"/>
@@ -5760,28 +6043,28 @@
     </row>
     <row r="4" spans="1:12" ht="239.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="60" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="C4" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="60" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="E4" s="60" t="s">
-        <v>112</v>
-      </c>
       <c r="F4" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G4" s="60" t="s">
         <v>29</v>
       </c>
       <c r="H4" s="60" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I4" s="61"/>
       <c r="J4" s="60"/>
@@ -5790,28 +6073,28 @@
     </row>
     <row r="5" spans="1:12" ht="221.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" s="60" t="s">
         <v>113</v>
       </c>
-      <c r="B5" s="60" t="s">
-        <v>114</v>
-      </c>
       <c r="C5" s="60" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="60" t="s">
         <v>103</v>
       </c>
-      <c r="E5" s="60" t="s">
-        <v>104</v>
-      </c>
       <c r="F5" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G5" s="60" t="s">
         <v>29</v>
       </c>
       <c r="H5" s="60" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I5" s="61"/>
       <c r="J5" s="60"/>
@@ -5820,28 +6103,28 @@
     </row>
     <row r="6" spans="1:12" ht="233.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="62" t="s">
         <v>115</v>
       </c>
-      <c r="B6" s="62" t="s">
+      <c r="C6" s="62" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" s="60" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="62" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="E6" s="60" t="s">
-        <v>117</v>
-      </c>
       <c r="F6" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G6" s="60" t="s">
         <v>29</v>
       </c>
       <c r="H6" s="62" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I6" s="61"/>
       <c r="J6" s="60"/>
@@ -5850,28 +6133,28 @@
     </row>
     <row r="7" spans="1:12" ht="207.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="60" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="E7" s="60" t="s">
-        <v>108</v>
-      </c>
       <c r="F7" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G7" s="60" t="s">
         <v>29</v>
       </c>
       <c r="H7" s="60" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I7" s="61"/>
       <c r="J7" s="60"/>
@@ -5880,28 +6163,28 @@
     </row>
     <row r="8" spans="1:12" ht="249.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="59" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="63" t="s">
         <v>120</v>
       </c>
-      <c r="B8" s="63" t="s">
+      <c r="C8" s="60" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" s="60" t="s">
         <v>121</v>
       </c>
-      <c r="C8" s="60" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="60" t="s">
-        <v>103</v>
-      </c>
-      <c r="E8" s="60" t="s">
-        <v>122</v>
-      </c>
       <c r="F8" s="60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G8" s="60" t="s">
         <v>29</v>
       </c>
       <c r="H8" s="63" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I8" s="61"/>
       <c r="J8" s="60"/>
@@ -5935,7 +6218,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B1" s="56" t="s">
         <v>12</v>
@@ -5944,7 +6227,7 @@
         <v>13</v>
       </c>
       <c r="D1" s="56" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E1" s="56" t="s">
         <v>15</v>
@@ -5956,10 +6239,10 @@
         <v>17</v>
       </c>
       <c r="H1" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="56" t="s">
         <v>98</v>
-      </c>
-      <c r="I1" s="56" t="s">
-        <v>99</v>
       </c>
       <c r="J1" s="56" t="s">
         <v>4</v>
@@ -5968,31 +6251,31 @@
     </row>
     <row r="2" spans="1:11" ht="210" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="54" t="s">
+      <c r="C2" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="54" t="s">
+      <c r="D2" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="D2" s="54" t="s">
+      <c r="E2" s="54" t="s">
         <v>90</v>
       </c>
-      <c r="E2" s="54" t="s">
+      <c r="F2" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="54" t="s">
+      <c r="G2" s="54" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="54" t="s">
+      <c r="H2" s="54" t="s">
         <v>93</v>
       </c>
-      <c r="H2" s="54" t="s">
+      <c r="I2" s="54" t="s">
         <v>94</v>
-      </c>
-      <c r="I2" s="54" t="s">
-        <v>95</v>
       </c>
       <c r="J2" s="54"/>
       <c r="K2" s="52"/>

</xml_diff>

<commit_message>
Design TCs for login and logout
Designed all the test cases for admin and user for login and logout features.
</commit_message>
<xml_diff>
--- a/5- Testing/Test Cases.xlsx
+++ b/5- Testing/Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Documents\GitHub\Car-Purchasing-App\5- Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4EC25A-6437-4F1F-BBD9-503CFD621BFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035815D7-4B37-4FC2-8FD2-5D875F4BE584}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="222">
   <si>
     <t>Module</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>Steps</t>
-  </si>
-  <si>
-    <t>Test Data</t>
   </si>
   <si>
     <t>Designed By</t>
@@ -345,95 +342,6 @@
     <t>Verify that user sees a pop-up message when there are no cars available for the entered brand name.</t>
   </si>
   <si>
-    <t>1_logout_user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Validate that the logout is working from the customer portal 
-</t>
-  </si>
-  <si>
-    <t>Functional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Register page is reachable.
-2. Edge Browser is available.
-3. Availability of test data for "UserID &amp; password".
-</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">
-1. Enter '</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00FF00"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>1305892</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>'
-in the user-id Field.
-2. Enter '</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF00FF00"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>12345ssss</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>' in the password field.
-3. Press the 'LOGIN' Button.</t>
-    </r>
-  </si>
-  <si>
-    <t>1- user-id : 1305892
-2- password : 12345ssss</t>
-  </si>
-  <si>
-    <t>Fouda</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>the user-id field should accept 
-the user-id and password move to the next 
-page after pressing
-'LOGOUT' successfully</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>PreCondition</t>
-  </si>
-  <si>
-    <t>Priotity</t>
-  </si>
-  <si>
-    <t>ER</t>
-  </si>
-  <si>
     <t>Brand Field(User)</t>
   </si>
   <si>
@@ -722,51 +630,16 @@
 2- User is registered in the system.</t>
   </si>
   <si>
-    <t>1. Open the login Page.
-2. enter "beshoy1@gmail.com" in the email field.
-3. enter "123456789" in the password field.
-4. Enter Login button.</t>
-  </si>
-  <si>
     <t>The home page should be displayed successfully to the user.</t>
   </si>
   <si>
-    <t>TC-Login-
-Cancel-12</t>
-  </si>
-  <si>
-    <t>Verify navigation to sign-up page when the user clicks on the sign-up button.</t>
-  </si>
-  <si>
-    <t>1. Open Login page.
-2.Click on the sign-up button.</t>
-  </si>
-  <si>
-    <t>The sign-up page should be displayed.</t>
-  </si>
-  <si>
     <t>Email Field (User)</t>
   </si>
   <si>
     <t>Verify error message will dissaper when the email field is left blank.</t>
   </si>
   <si>
-    <t>1. Open the login Page.
-2. enter "   " in the email field.
-3. enter "123456789" in the password field.
-4. Enter Login button.</t>
-  </si>
-  <si>
     <t>An error message should be displayed "Please fill out this field".</t>
-  </si>
-  <si>
-    <t>Verify that an error message should be displayed for the invalid email format.</t>
-  </si>
-  <si>
-    <t>1. Open the login Page.
-2. enter " beshoy1gmail.com  " in the email field.
-3. enter "123456789" in the password field.
-4. Enter Login button.</t>
   </si>
   <si>
     <t>An error message should be displayed "Invalid email or password".</t>
@@ -778,73 +651,323 @@
 4. Enter Login button.</t>
   </si>
   <si>
+    <t>Verify that an error message should be displayed for the invalid email format(special character).</t>
+  </si>
+  <si>
+    <t>Verify that an error message should be displayed for the invalid email format(space before .com).</t>
+  </si>
+  <si>
+    <t>Verify that an error message should be displayed for the invalid email format(space btween the mail).</t>
+  </si>
+  <si>
+    <t>Verify that an error message should be displayed for unregistered email with correct password.</t>
+  </si>
+  <si>
+    <t>Verify that an error message should be displayed for un registered email and password.</t>
+  </si>
+  <si>
+    <t>Verify that an error message should be displayed for the invalid email format(without@).</t>
+  </si>
+  <si>
+    <t>Verify that an error message should be displayed for the invalid email format(without .com).</t>
+  </si>
+  <si>
+    <t>Paaword Field(User)</t>
+  </si>
+  <si>
+    <t>Verify that an error message should be displayed for the invalid email format (without @ &amp; .com).</t>
+  </si>
+  <si>
+    <t>Verify that an error message should be displayed for correct email with incorrect password.</t>
+  </si>
+  <si>
+    <t>1. Open the login Page.
+2. enter " beshoy1@gmail.com " in the email field.
+3. enter "123456780" in the password field.
+4. Press Login button.</t>
+  </si>
+  <si>
+    <t>1. Open the login Page.
+2. enter "beshoy1@gmail.com" in the email field.
+3. enter "123456789" in the password field.
+4. Press Login button.</t>
+  </si>
+  <si>
+    <t>1. Open the login Page.
+2. enter "   " in the email field.
+3. enter "123456789" in the password field.
+4. press Login button.</t>
+  </si>
+  <si>
+    <t>1. Open the login Page.
+2. enter " beshoy1gmail.com  " in the email field.
+3. enter "123456789" in the password field.
+4. press Login button.</t>
+  </si>
+  <si>
+    <t>1. Open the login Page.
+2. enter " beshoy1" in the email field.
+3. enter "123456789" in the password field.
+4. press Login button.</t>
+  </si>
+  <si>
     <t>1. Open the login Page.
 2. enter " beshoy1@!gmail.com " in the email field.
 3. enter "123456789" in the password field.
-4. Enter Login button.</t>
-  </si>
-  <si>
-    <t>Verify that an error message should be displayed for the invalid email format(special character).</t>
-  </si>
-  <si>
-    <t>Verify that an error message should be displayed for the invalid email format(space before .com).</t>
-  </si>
-  <si>
-    <t>Verify that an error message should be displayed for the invalid email format(space btween the mail).</t>
+4. press Login button.</t>
+  </si>
+  <si>
+    <t>1. Open the login Page.
+2. enter " beshoy1@gmail .com " in the email field.
+3. enter "123456789" in the password field.
+4. press Login button.</t>
   </si>
   <si>
     <t>1. Open the login Page.
 2. enter " bes hoy1@gmail.com " in the email field.
 3. enter "123456789" in the password field.
-4. Enter Login button.</t>
-  </si>
-  <si>
-    <t>1. Open the login Page.
-2. enter " beshoy1@gmail .com " in the email field.
-3. enter "123456789" in the password field.
-4. Enter Login button.</t>
+4. press Login button.</t>
   </si>
   <si>
     <t>1. Open the login Page.
 2. enter " beshoy2@gmail.com " in the email field.
 3. enter "123456789" in the password field.
-4. Enter Login button.</t>
-  </si>
-  <si>
-    <t>Verify that an error message should be displayed for unregistered email with correct password.</t>
-  </si>
-  <si>
-    <t>Verify that an error message should be displayed forcorrect email with incorrect password.</t>
-  </si>
-  <si>
-    <t>1. Open the login Page.
-2. enter " beshoy1@gmail.com " in the email field.
-3. enter "123456780" in the password field.
-4. Enter Login button.</t>
-  </si>
-  <si>
-    <t>Verify that an error message should be displayed for un registered email and password.</t>
+4. press Login button.</t>
   </si>
   <si>
     <t>1. Open the login Page.
 2. enter " beshoy2@gmail.com " in the email field.
 3. enter "123456780" in the password field.
-4. Enter Login button.</t>
-  </si>
-  <si>
-    <t>Verify that an error message should be displayed for the invalid email format(without@).</t>
+4. press Login button.</t>
+  </si>
+  <si>
+    <t>Verify error message 'll be displayed when the password field is left blank.</t>
   </si>
   <si>
     <t>1. Open the login Page.
-2. enter " beshoy1" in the email field.
-3. enter "123456789" in the password field.
-4. Enter Login button.</t>
-  </si>
-  <si>
-    <t>Verify that an error message should be displayed for the invalid email format(without .com).</t>
-  </si>
-  <si>
-    <t>Paaword Field(User)</t>
+2. enter " beshoy1@gmail.com " in the email field.
+3. enter "   " in the password field.
+4. press Login button.</t>
+  </si>
+  <si>
+    <t>Verify error message should be displayed when the 
+password 
+length is less than 8 characters.</t>
+  </si>
+  <si>
+    <t>1. Open the login Page.
+2. enter " beshoy1@gmail.com " in the email field.
+3. enter " 1234567 " in the password field.
+4. press Login button.</t>
+  </si>
+  <si>
+    <t>The password field, should display any input as asterisk.</t>
+  </si>
+  <si>
+    <t>Verify that the password is masked 
+( displayed as asterisks"***")</t>
+  </si>
+  <si>
+    <t>1. Open the login Page.
+2. press sign-up button.</t>
+  </si>
+  <si>
+    <t>Verify navigation to  
+ sign-up page  when the user clicks
+on the sign-up button.</t>
+  </si>
+  <si>
+    <t>The sThe system should let the user navigate to the sign-up page.</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-User-02</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-User-01</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-User-03</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-User-04</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-User-05</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-User-06</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-User-07</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-User-08</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-User-09</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-User-10</t>
+  </si>
+  <si>
+    <t>TC-PasswordLogin
+-User-11</t>
+  </si>
+  <si>
+    <t>TC-PasswordLogin
+-User-12</t>
+  </si>
+  <si>
+    <t>TC-PasswordLogin
+-User-13</t>
+  </si>
+  <si>
+    <t>TC-Login
+-Admin-00</t>
+  </si>
+  <si>
+    <t>1- browser is available 
+2- Admin is registered in the system.</t>
+  </si>
+  <si>
+    <t>The home page should be displayed successfully to the admin.</t>
+  </si>
+  <si>
+    <t>The system should let the admin navigate to the sign-up page.</t>
+  </si>
+  <si>
+    <t>Verify navigation to  
+ sign-up page  when the admin clicks
+on the sign-up button.</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-Admin-01</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-Admin-02</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-Admin-03</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-Admin-04</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-Admin-05</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-Admin-06</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-Admin-07</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-Admin-08</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-Admin-09</t>
+  </si>
+  <si>
+    <t>TC-EmailLogin
+-Admin-10</t>
+  </si>
+  <si>
+    <t>TC-PasswordLogin
+-Admin-11</t>
+  </si>
+  <si>
+    <t>TC-PasswordLogin
+-Admin-12</t>
+  </si>
+  <si>
+    <t>TC-Signup
+-Admin-14</t>
+  </si>
+  <si>
+    <t>TC-Signup
+-User-14</t>
+  </si>
+  <si>
+    <t>Paaword Field(Admin)</t>
+  </si>
+  <si>
+    <t>TC-Logout
+-User-00</t>
+  </si>
+  <si>
+    <t>Verify successful logout for a user.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Click Logout button.</t>
+  </si>
+  <si>
+    <t>The user should be  successfully logged out and the login page should be displayed.</t>
+  </si>
+  <si>
+    <t>User (Logout)</t>
+  </si>
+  <si>
+    <t>TC-Logout
+-Admin-00</t>
+  </si>
+  <si>
+    <t>Verify successful logout for a admin.</t>
+  </si>
+  <si>
+    <t>The admin should be  successfully logged out and the login page should be displayed.</t>
+  </si>
+  <si>
+    <t>Admin(Logout)</t>
+  </si>
+  <si>
+    <t>Verify that the user can't access the home page after logout.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ Click Logout button on the home page.
+</t>
+  </si>
+  <si>
+    <t>TC-Logout
+-User-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+ 1.Click Logout button on the home page.
+2. Click "go back" button in the browser.</t>
+  </si>
+  <si>
+    <t>The user should not be able to go to the home page before logging in again.</t>
+  </si>
+  <si>
+    <t>TC-Logout
+-Admin-01</t>
+  </si>
+  <si>
+    <t>Verify that the admin can't access the home page after logout.</t>
+  </si>
+  <si>
+    <t>The admin should not be able to go to the home page before logging in again.</t>
   </si>
 </sst>
 </file>
@@ -978,25 +1101,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF00FF00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="20"/>
       <color theme="2"/>
@@ -1017,8 +1121,27 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="26"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1103,14 +1226,8 @@
         <bgColor rgb="FFFF00FF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF073763"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1214,81 +1331,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF434343"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF434343"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF434343"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF434343"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF434343"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FF434343"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -1343,11 +1385,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1464,116 +1589,154 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
@@ -5019,8 +5182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7E3B47-1521-4401-9600-50F8B310637B}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView topLeftCell="G14" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I15"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5041,544 +5204,544 @@
   <sheetData>
     <row r="1" spans="1:13" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="51" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="60" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="61" t="s">
+      <c r="M1" s="47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="207" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="64"/>
+      <c r="B2" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="60" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="60" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="60" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" s="60" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="60" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="60" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="60" t="s">
+      <c r="E2" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="60" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" s="60" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="207" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45"/>
-      <c r="B2" s="52" t="s">
+      <c r="G2" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="41"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="54"/>
+    </row>
+    <row r="3" spans="1:13" ht="175.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="65"/>
+      <c r="B3" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="E3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="49" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="50" t="s">
+      <c r="J3" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="56"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="54"/>
+    </row>
+    <row r="4" spans="1:13" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="A4" s="65"/>
+      <c r="B4" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="50"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="54"/>
+    </row>
+    <row r="5" spans="1:13" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="A5" s="65"/>
+      <c r="B5" s="69"/>
+      <c r="C5" s="40" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="I2" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="65" t="s">
+      <c r="E5" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="K2" s="50"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="67"/>
-    </row>
-    <row r="3" spans="1:13" ht="175.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46"/>
-      <c r="B3" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="62" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="64" t="s">
+      <c r="I5" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="50"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="54"/>
+    </row>
+    <row r="6" spans="1:13" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="A6" s="65"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="H6" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="I6" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="K6" s="50"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="54"/>
+    </row>
+    <row r="7" spans="1:13" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="65"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="40" t="s">
+        <v>123</v>
+      </c>
+      <c r="D7" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="J3" s="68" t="s">
-        <v>49</v>
-      </c>
-      <c r="K3" s="69"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="67"/>
-    </row>
-    <row r="4" spans="1:13" ht="142.5" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
-      <c r="B4" s="53" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="62" t="s">
+      <c r="E7" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="64" t="s">
+      <c r="G7" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="50" t="s">
+      <c r="H7" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="I7" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="K7" s="50"/>
+      <c r="L7" s="57"/>
+      <c r="M7" s="54"/>
+    </row>
+    <row r="8" spans="1:13" ht="128.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="65"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="40" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="50" t="s">
-        <v>45</v>
-      </c>
-      <c r="I4" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="68" t="s">
-        <v>46</v>
-      </c>
-      <c r="K4" s="63"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="67"/>
-    </row>
-    <row r="5" spans="1:13" ht="142.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="46"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="50" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="64" t="s">
+      <c r="E8" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="50" t="s">
+      <c r="H8" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="K8" s="50"/>
+      <c r="L8" s="57"/>
+      <c r="M8" s="54"/>
+    </row>
+    <row r="9" spans="1:13" ht="162" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="65"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="50" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="K5" s="63"/>
-      <c r="L5" s="70"/>
-      <c r="M5" s="67"/>
-    </row>
-    <row r="6" spans="1:13" ht="142.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="46"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="49" t="s">
-        <v>136</v>
-      </c>
-      <c r="D6" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="50" t="s">
-        <v>126</v>
-      </c>
-      <c r="F6" s="64" t="s">
+      <c r="E9" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="G6" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="50" t="s">
-        <v>127</v>
-      </c>
-      <c r="I6" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="50" t="s">
+      <c r="H9" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="I9" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="K9" s="50"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="54"/>
+    </row>
+    <row r="10" spans="1:13" ht="183" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="65"/>
+      <c r="B10" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="40" t="s">
         <v>128</v>
       </c>
-      <c r="K6" s="63"/>
-      <c r="L6" s="70"/>
-      <c r="M6" s="67"/>
-    </row>
-    <row r="7" spans="1:13" ht="142.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="46"/>
-      <c r="B7" s="54"/>
-      <c r="C7" s="49" t="s">
-        <v>137</v>
-      </c>
-      <c r="D7" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="50" t="s">
-        <v>114</v>
-      </c>
-      <c r="F7" s="64" t="s">
+      <c r="D10" s="40">
+        <v>0</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>104</v>
+      </c>
+      <c r="F10" s="38"/>
+      <c r="G10" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="G7" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="50" t="s">
-        <v>115</v>
-      </c>
-      <c r="I7" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="50" t="s">
-        <v>116</v>
-      </c>
-      <c r="K7" s="63"/>
-      <c r="L7" s="70"/>
-      <c r="M7" s="67"/>
-    </row>
-    <row r="8" spans="1:13" ht="142.5" x14ac:dyDescent="0.2">
-      <c r="A8" s="46"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="49" t="s">
-        <v>138</v>
-      </c>
-      <c r="D8" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="50" t="s">
-        <v>129</v>
-      </c>
-      <c r="F8" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="H8" s="50" t="s">
-        <v>130</v>
-      </c>
-      <c r="I8" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="50" t="s">
-        <v>128</v>
-      </c>
-      <c r="K8" s="63"/>
-      <c r="L8" s="70"/>
-      <c r="M8" s="67"/>
-    </row>
-    <row r="9" spans="1:13" ht="162" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="46"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="49" t="s">
-        <v>139</v>
-      </c>
-      <c r="D9" s="62" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="50" t="s">
-        <v>131</v>
-      </c>
-      <c r="F9" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="50" t="s">
-        <v>132</v>
-      </c>
-      <c r="I9" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="50" t="s">
-        <v>133</v>
-      </c>
-      <c r="K9" s="63"/>
-      <c r="L9" s="70"/>
-      <c r="M9" s="67"/>
-    </row>
-    <row r="10" spans="1:13" ht="183" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="46"/>
-      <c r="B10" s="55" t="s">
-        <v>117</v>
-      </c>
-      <c r="C10" s="49" t="s">
-        <v>142</v>
-      </c>
-      <c r="D10" s="49">
-        <v>0</v>
-      </c>
-      <c r="E10" s="39" t="s">
-        <v>118</v>
-      </c>
-      <c r="F10" s="38"/>
-      <c r="G10" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="H10" s="50" t="s">
-        <v>119</v>
-      </c>
-      <c r="I10" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="68" t="s">
-        <v>120</v>
+      <c r="H10" s="41" t="s">
+        <v>105</v>
+      </c>
+      <c r="I10" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="55" t="s">
+        <v>106</v>
       </c>
       <c r="K10" s="36"/>
       <c r="L10" s="36"/>
       <c r="M10" s="36"/>
     </row>
     <row r="11" spans="1:13" ht="183" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="46"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="49" t="s">
-        <v>143</v>
-      </c>
-      <c r="D11" s="49">
+      <c r="A11" s="65"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="D11" s="40">
         <v>0</v>
       </c>
       <c r="E11" s="39" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="F11" s="38"/>
-      <c r="G11" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="50" t="s">
-        <v>122</v>
-      </c>
-      <c r="I11" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" s="68" t="s">
-        <v>123</v>
+      <c r="G11" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="I11" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="55" t="s">
+        <v>109</v>
       </c>
       <c r="K11" s="36"/>
       <c r="L11" s="36"/>
       <c r="M11" s="36"/>
     </row>
     <row r="12" spans="1:13" ht="183" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="46"/>
-      <c r="B12" s="56"/>
-      <c r="C12" s="49" t="s">
-        <v>144</v>
-      </c>
-      <c r="D12" s="49">
+      <c r="A12" s="65"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" s="40">
         <v>0</v>
       </c>
       <c r="E12" s="39" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="F12" s="38"/>
-      <c r="G12" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="H12" s="50" t="s">
-        <v>135</v>
-      </c>
-      <c r="I12" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="68" t="s">
-        <v>123</v>
+      <c r="G12" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="I12" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="J12" s="55" t="s">
+        <v>109</v>
       </c>
       <c r="K12" s="36"/>
       <c r="L12" s="36"/>
       <c r="M12" s="36"/>
     </row>
     <row r="13" spans="1:13" ht="157.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="46"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="49" t="s">
-        <v>145</v>
-      </c>
-      <c r="D13" s="49">
+      <c r="A13" s="65"/>
+      <c r="B13" s="72"/>
+      <c r="C13" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="40">
         <v>0</v>
       </c>
       <c r="E13" s="39" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="F13" s="38"/>
-      <c r="G13" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="50" t="s">
-        <v>125</v>
-      </c>
-      <c r="I13" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="J13" s="68" t="s">
-        <v>123</v>
+      <c r="G13" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="I13" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="55" t="s">
+        <v>109</v>
       </c>
       <c r="K13" s="36"/>
       <c r="L13" s="36"/>
       <c r="M13" s="36"/>
     </row>
     <row r="14" spans="1:13" ht="130.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="46"/>
-      <c r="B14" s="58" t="s">
+      <c r="A14" s="65"/>
+      <c r="B14" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="40" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" s="58">
+        <v>6.1</v>
+      </c>
+      <c r="E14" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="49" t="s">
-        <v>140</v>
-      </c>
-      <c r="D14" s="71">
-        <v>6.1</v>
-      </c>
-      <c r="E14" s="50" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="50" t="s">
+      <c r="F14" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="I14" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="I14" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="J14" s="72" t="s">
-        <v>54</v>
-      </c>
-      <c r="K14" s="63"/>
-      <c r="L14" s="70"/>
-      <c r="M14" s="67"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="57"/>
+      <c r="M14" s="54"/>
     </row>
     <row r="15" spans="1:13" ht="84.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="48"/>
-      <c r="B15" s="59" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="49" t="s">
-        <v>141</v>
-      </c>
-      <c r="D15" s="49" t="s">
-        <v>27</v>
+      <c r="A15" s="66"/>
+      <c r="B15" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>26</v>
       </c>
       <c r="E15" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="38"/>
+      <c r="G15" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="38"/>
-      <c r="G15" s="50" t="s">
+      <c r="H15" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="H15" s="37" t="s">
+      <c r="I15" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="37" t="s">
         <v>63</v>
-      </c>
-      <c r="I15" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15" s="37" t="s">
-        <v>64</v>
       </c>
       <c r="K15" s="36"/>
       <c r="L15" s="36"/>
       <c r="M15" s="36"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="46"/>
+      <c r="A16" s="65"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="46"/>
+      <c r="A17" s="65"/>
     </row>
     <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="46"/>
-      <c r="E18" s="73"/>
+      <c r="A18" s="65"/>
+      <c r="E18" s="60"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="46"/>
+      <c r="A19" s="65"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="46"/>
+      <c r="A20" s="65"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="46"/>
+      <c r="A21" s="65"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="46"/>
+      <c r="A22" s="65"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="46"/>
+      <c r="A23" s="65"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="46"/>
+      <c r="A24" s="65"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="46"/>
+      <c r="A25" s="65"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="46"/>
+      <c r="A26" s="65"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="46"/>
+      <c r="A27" s="65"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="46"/>
+      <c r="A28" s="65"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="46"/>
+      <c r="A29" s="65"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="46"/>
+      <c r="A30" s="65"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="46"/>
+      <c r="A31" s="65"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="46"/>
+      <c r="A32" s="65"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="46"/>
+      <c r="A33" s="65"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="46"/>
+      <c r="A34" s="65"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="46"/>
+      <c r="A35" s="65"/>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="47"/>
+      <c r="A36" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5616,16 +5779,16 @@
   <sheetData>
     <row r="1" spans="1:13" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" s="24" t="s">
         <v>12</v>
@@ -5640,166 +5803,166 @@
         <v>15</v>
       </c>
       <c r="I1" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="K1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="24" t="s">
-        <v>19</v>
-      </c>
       <c r="L1" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M1" s="24" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="207.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45"/>
+      <c r="A2" s="64"/>
       <c r="B2" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="E2" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="F2" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="26" t="s">
-        <v>58</v>
-      </c>
       <c r="I2" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J2" s="32" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="K2" s="26"/>
       <c r="L2" s="21"/>
       <c r="M2" s="22"/>
     </row>
     <row r="3" spans="1:13" ht="220.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="46"/>
+      <c r="A3" s="65"/>
       <c r="B3" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="34" t="s">
         <v>65</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="E3" s="34" t="s">
-        <v>66</v>
       </c>
       <c r="F3" s="30"/>
       <c r="G3" s="35" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H3" s="37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I3" s="38"/>
       <c r="J3" s="39" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="K3" s="36"/>
       <c r="L3" s="36"/>
       <c r="M3" s="36"/>
     </row>
     <row r="4" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
+      <c r="A4" s="65"/>
     </row>
     <row r="5" spans="1:13" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="46"/>
+      <c r="A5" s="65"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="46"/>
+      <c r="A6" s="65"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="46"/>
+      <c r="A7" s="65"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="46"/>
+      <c r="A8" s="65"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="46"/>
+      <c r="A9" s="65"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="46"/>
+      <c r="A10" s="65"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="46"/>
+      <c r="A11" s="65"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="46"/>
+      <c r="A12" s="65"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="46"/>
+      <c r="A13" s="65"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="46"/>
+      <c r="A14" s="65"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="46"/>
+      <c r="A15" s="65"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="46"/>
+      <c r="A16" s="65"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="46"/>
+      <c r="A17" s="65"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="46"/>
+      <c r="A18" s="65"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="46"/>
+      <c r="A19" s="65"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="46"/>
+      <c r="A20" s="65"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="46"/>
+      <c r="A21" s="65"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="46"/>
+      <c r="A22" s="65"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="46"/>
+      <c r="A23" s="65"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="46"/>
+      <c r="A24" s="65"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="46"/>
+      <c r="A25" s="65"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="46"/>
+      <c r="A26" s="65"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="46"/>
+      <c r="A27" s="65"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="46"/>
+      <c r="A28" s="65"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="46"/>
+      <c r="A29" s="65"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="46"/>
+      <c r="A30" s="65"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="47"/>
+      <c r="A31" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5834,16 +5997,16 @@
   <sheetData>
     <row r="1" spans="1:13" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C1" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" s="24" t="s">
         <v>12</v>
@@ -5858,140 +6021,140 @@
         <v>15</v>
       </c>
       <c r="I1" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="K1" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="24" t="s">
-        <v>19</v>
-      </c>
       <c r="L1" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M1" s="24" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="174.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="45"/>
+      <c r="A2" s="64"/>
       <c r="B2" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="E2" s="26" t="s">
+      <c r="F2" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="F2" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" s="26" t="s">
+      <c r="I2" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="34" t="s">
         <v>71</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="34" t="s">
-        <v>72</v>
       </c>
       <c r="K2" s="26"/>
       <c r="L2" s="21"/>
       <c r="M2" s="22"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="46"/>
+      <c r="A3" s="65"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="46"/>
+      <c r="A4" s="65"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="46"/>
+      <c r="A5" s="65"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="46"/>
+      <c r="A6" s="65"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="46"/>
+      <c r="A7" s="65"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="46"/>
+      <c r="A8" s="65"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" s="46"/>
+      <c r="A9" s="65"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="46"/>
+      <c r="A10" s="65"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" s="46"/>
+      <c r="A11" s="65"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="46"/>
+      <c r="A12" s="65"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="46"/>
+      <c r="A13" s="65"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" s="46"/>
+      <c r="A14" s="65"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" s="46"/>
+      <c r="A15" s="65"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16" s="46"/>
+      <c r="A16" s="65"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="46"/>
+      <c r="A17" s="65"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="46"/>
+      <c r="A18" s="65"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="46"/>
+      <c r="A19" s="65"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="46"/>
+      <c r="A20" s="65"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="46"/>
+      <c r="A21" s="65"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="46"/>
+      <c r="A22" s="65"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="46"/>
+      <c r="A23" s="65"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="46"/>
+      <c r="A24" s="65"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="46"/>
+      <c r="A25" s="65"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="46"/>
+      <c r="A26" s="65"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="46"/>
+      <c r="A27" s="65"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="46"/>
+      <c r="A28" s="65"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="46"/>
+      <c r="A29" s="65"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="46"/>
+      <c r="A30" s="65"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="47"/>
+      <c r="A31" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6005,8 +6168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D229A3A4-4F9D-42AB-80C8-669754DC12C3}">
   <dimension ref="A1:L9"/>
   <sheetViews>
-    <sheetView topLeftCell="B8" workbookViewId="0">
-      <selection sqref="A1:L9"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6026,287 +6189,287 @@
   <sheetData>
     <row r="1" spans="1:12" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="61" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="74" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="75" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="74" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="74" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="74" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="74" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="74" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="74" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="74" t="s">
+      <c r="L1" s="61" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="179.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="74" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="179.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="53" t="s">
-        <v>91</v>
-      </c>
-      <c r="B2" s="49" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="50" t="s">
+      <c r="F2" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="E2" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="G2" s="50" t="s">
+      <c r="H2" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="39" t="s">
+      <c r="J2" s="41"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="54"/>
+    </row>
+    <row r="3" spans="1:12" ht="148.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="69"/>
+      <c r="B3" s="40" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="J2" s="50"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="67"/>
-    </row>
-    <row r="3" spans="1:12" ht="148.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="54"/>
-      <c r="B3" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="49" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="50" t="s">
-        <v>95</v>
-      </c>
-      <c r="H3" s="64" t="s">
-        <v>25</v>
+      <c r="E3" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" s="51" t="s">
+        <v>24</v>
       </c>
       <c r="I3" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="J3" s="50"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="67"/>
+        <v>82</v>
+      </c>
+      <c r="J3" s="41"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="54"/>
     </row>
     <row r="4" spans="1:12" ht="114" x14ac:dyDescent="0.2">
-      <c r="A4" s="53" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="C4" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="50" t="s">
-        <v>99</v>
-      </c>
-      <c r="E4" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="50" t="s">
-        <v>100</v>
-      </c>
-      <c r="H4" s="64" t="s">
-        <v>25</v>
+      <c r="A4" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="41" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="51" t="s">
+        <v>24</v>
       </c>
       <c r="I4" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="J4" s="50"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="67"/>
+        <v>87</v>
+      </c>
+      <c r="J4" s="41"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="54"/>
     </row>
     <row r="5" spans="1:12" ht="114" x14ac:dyDescent="0.2">
-      <c r="A5" s="54"/>
-      <c r="B5" s="49" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="49" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="50" t="s">
-        <v>103</v>
-      </c>
-      <c r="E5" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="50" t="s">
-        <v>100</v>
-      </c>
-      <c r="H5" s="64" t="s">
-        <v>25</v>
+      <c r="A5" s="69"/>
+      <c r="B5" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="C5" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" s="51" t="s">
+        <v>24</v>
       </c>
       <c r="I5" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="J5" s="63"/>
+        <v>82</v>
+      </c>
+      <c r="J5" s="50"/>
       <c r="K5" s="36"/>
       <c r="L5" s="36"/>
     </row>
     <row r="6" spans="1:12" ht="114" x14ac:dyDescent="0.2">
-      <c r="A6" s="53" t="s">
-        <v>104</v>
-      </c>
-      <c r="B6" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="50" t="s">
-        <v>106</v>
-      </c>
-      <c r="E6" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="G6" s="50" t="s">
+      <c r="A6" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="E6" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="39" t="s">
         <v>75</v>
       </c>
-      <c r="H6" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="J6" s="50"/>
-      <c r="K6" s="70"/>
-      <c r="L6" s="67"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="54"/>
     </row>
     <row r="7" spans="1:12" ht="114" x14ac:dyDescent="0.2">
-      <c r="A7" s="54"/>
-      <c r="B7" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="C7" s="49" t="s">
+      <c r="A7" s="69"/>
+      <c r="B7" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="D7" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="E7" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="50" t="s">
+      <c r="E7" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="H7" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>82</v>
+      </c>
+      <c r="J7" s="41"/>
+      <c r="K7" s="57"/>
+      <c r="L7" s="54"/>
+    </row>
+    <row r="8" spans="1:12" ht="114" x14ac:dyDescent="0.2">
+      <c r="A8" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="H7" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="39" t="s">
+      <c r="B8" s="40" t="s">
         <v>96</v>
       </c>
-      <c r="J7" s="50"/>
-      <c r="K7" s="70"/>
-      <c r="L7" s="67"/>
-    </row>
-    <row r="8" spans="1:12" ht="114" x14ac:dyDescent="0.2">
-      <c r="A8" s="53" t="s">
-        <v>109</v>
-      </c>
-      <c r="B8" s="49" t="s">
-        <v>110</v>
-      </c>
-      <c r="C8" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="50" t="s">
-        <v>111</v>
-      </c>
-      <c r="E8" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="50" t="s">
-        <v>100</v>
-      </c>
-      <c r="H8" s="64" t="s">
-        <v>25</v>
+      <c r="C8" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="H8" s="51" t="s">
+        <v>24</v>
       </c>
       <c r="I8" s="39" t="s">
-        <v>101</v>
-      </c>
-      <c r="J8" s="50"/>
-      <c r="K8" s="70"/>
-      <c r="L8" s="67"/>
+        <v>87</v>
+      </c>
+      <c r="J8" s="41"/>
+      <c r="K8" s="57"/>
+      <c r="L8" s="54"/>
     </row>
     <row r="9" spans="1:12" ht="114" x14ac:dyDescent="0.2">
-      <c r="A9" s="54"/>
-      <c r="B9" s="49" t="s">
-        <v>112</v>
-      </c>
-      <c r="C9" s="49" t="s">
-        <v>94</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" s="64" t="s">
+      <c r="A9" s="69"/>
+      <c r="B9" s="40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="E9" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="50" t="s">
-        <v>100</v>
-      </c>
-      <c r="H9" s="64" t="s">
-        <v>25</v>
+      <c r="G9" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="51" t="s">
+        <v>24</v>
       </c>
       <c r="I9" s="39" t="s">
-        <v>96</v>
-      </c>
-      <c r="J9" s="63"/>
+        <v>82</v>
+      </c>
+      <c r="J9" s="50"/>
       <c r="K9" s="36"/>
       <c r="L9" s="36"/>
     </row>
@@ -6323,496 +6486,928 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E3E3723-9A66-41B9-B3EE-9ACDC170719F}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection sqref="A1:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" customWidth="1"/>
     <col min="6" max="6" width="23.7109375" customWidth="1"/>
     <col min="7" max="7" width="34.42578125" customWidth="1"/>
     <col min="8" max="8" width="21.42578125" customWidth="1"/>
     <col min="9" max="9" width="27.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="47.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="42" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="74" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="75" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="74" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="74" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="74" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="74" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="74" t="s">
-        <v>17</v>
-      </c>
-      <c r="I1" s="74" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="74" t="s">
+      <c r="L1" s="47" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="204.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="63" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="40">
+        <v>0</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="74" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="74" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="204.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="49" t="s">
+      <c r="F2" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="J2" s="41"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="54"/>
+    </row>
+    <row r="3" spans="1:12" ht="239.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="40"/>
+      <c r="D3" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>155</v>
+      </c>
+      <c r="H3" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="J3" s="41"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="54"/>
+    </row>
+    <row r="4" spans="1:12" ht="239.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="69"/>
+      <c r="B4" s="40" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" s="40"/>
+      <c r="D4" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="C2" s="49">
-        <v>0</v>
-      </c>
-      <c r="D2" s="50" t="s">
+      <c r="E4" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="H4" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J4" s="41"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="36"/>
+    </row>
+    <row r="5" spans="1:12" ht="239.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="69"/>
+      <c r="B5" s="40" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" s="40"/>
+      <c r="D5" s="41" t="s">
+        <v>151</v>
+      </c>
+      <c r="E5" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="H5" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J5" s="36"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="36"/>
+    </row>
+    <row r="6" spans="1:12" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="69"/>
+      <c r="B6" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" s="40"/>
+      <c r="D6" s="41" t="s">
         <v>149</v>
       </c>
-      <c r="E2" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="50" t="s">
+      <c r="E6" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G6" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="H6" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+    </row>
+    <row r="7" spans="1:12" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="45"/>
+      <c r="B7" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="40"/>
+      <c r="D7" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="E7" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G7" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="H7" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="36"/>
+    </row>
+    <row r="8" spans="1:12" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="45"/>
+      <c r="B8" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="40"/>
+      <c r="D8" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="E8" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G8" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="H8" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J8" s="36"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="36"/>
+    </row>
+    <row r="9" spans="1:12" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="45"/>
+      <c r="B9" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" s="40"/>
+      <c r="D9" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G9" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="H9" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J9" s="36"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="36"/>
+    </row>
+    <row r="10" spans="1:12" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="45"/>
+      <c r="B10" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" s="40"/>
+      <c r="D10" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G10" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="H10" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
+    </row>
+    <row r="11" spans="1:12" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="45"/>
+      <c r="B11" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="C11" s="40"/>
+      <c r="D11" s="41" t="s">
+        <v>152</v>
+      </c>
+      <c r="E11" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G11" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="H11" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+    </row>
+    <row r="12" spans="1:12" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="45"/>
+      <c r="B12" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" s="40"/>
+      <c r="D12" s="41" t="s">
+        <v>147</v>
+      </c>
+      <c r="E12" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="41" t="s">
+        <v>162</v>
+      </c>
+      <c r="H12" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
+    </row>
+    <row r="13" spans="1:12" ht="233.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="75" t="s">
         <v>150</v>
       </c>
-      <c r="G2" s="50" t="s">
+      <c r="B13" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="H13" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="J13" s="41"/>
+      <c r="K13" s="57"/>
+      <c r="L13" s="54"/>
+    </row>
+    <row r="14" spans="1:12" ht="207.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="76"/>
+      <c r="B14" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="C14" s="40"/>
+      <c r="D14" s="77" t="s">
+        <v>165</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="G14" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="H14" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J14" s="41"/>
+      <c r="K14" s="57"/>
+      <c r="L14" s="54"/>
+    </row>
+    <row r="15" spans="1:12" ht="207.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="45"/>
+      <c r="B15" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="C15" s="40"/>
+      <c r="D15" s="77" t="s">
+        <v>168</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="G15" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="H15" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I15" s="39" t="s">
+        <v>167</v>
+      </c>
+      <c r="J15" s="41"/>
+      <c r="K15" s="57"/>
+      <c r="L15" s="54"/>
+    </row>
+    <row r="16" spans="1:12" ht="130.5" x14ac:dyDescent="0.2">
+      <c r="A16" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" s="58"/>
+      <c r="D16" s="74" t="s">
+        <v>170</v>
+      </c>
+      <c r="E16" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="H16" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I16" s="74" t="s">
+        <v>171</v>
+      </c>
+      <c r="J16" s="50"/>
+      <c r="K16" s="57"/>
+      <c r="L16" s="54"/>
+    </row>
+    <row r="17" spans="1:12" ht="108" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="78" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="C17" s="40"/>
+      <c r="D17" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>154</v>
+      </c>
+      <c r="H17" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I17" s="39" t="s">
+        <v>187</v>
+      </c>
+      <c r="J17" s="41"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="54"/>
+    </row>
+    <row r="18" spans="1:12" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="82" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>190</v>
+      </c>
+      <c r="C18" s="40"/>
+      <c r="D18" s="41" t="s">
+        <v>139</v>
+      </c>
+      <c r="E18" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="G18" s="41" t="s">
+        <v>155</v>
+      </c>
+      <c r="H18" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="J18" s="41"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="54"/>
+    </row>
+    <row r="19" spans="1:12" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="83"/>
+      <c r="B19" s="40" t="s">
+        <v>191</v>
+      </c>
+      <c r="C19" s="40"/>
+      <c r="D19" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="E19" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="G19" s="41" t="s">
+        <v>156</v>
+      </c>
+      <c r="H19" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J19" s="41"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="36"/>
+    </row>
+    <row r="20" spans="1:12" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A20" s="83"/>
+      <c r="B20" s="40" t="s">
+        <v>192</v>
+      </c>
+      <c r="C20" s="40"/>
+      <c r="D20" s="41" t="s">
         <v>151</v>
       </c>
-      <c r="H2" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="39" t="s">
+      <c r="E20" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="F20" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="H20" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I20" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36"/>
+    </row>
+    <row r="21" spans="1:12" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="83"/>
+      <c r="B21" s="40" t="s">
+        <v>193</v>
+      </c>
+      <c r="C21" s="40"/>
+      <c r="D21" s="41" t="s">
+        <v>149</v>
+      </c>
+      <c r="E21" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="F21" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="G21" s="41" t="s">
+        <v>142</v>
+      </c>
+      <c r="H21" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I21" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+    </row>
+    <row r="22" spans="1:12" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="83"/>
+      <c r="B22" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="C22" s="40"/>
+      <c r="D22" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="E22" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="G22" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="H22" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J22" s="36"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="36"/>
+    </row>
+    <row r="23" spans="1:12" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="83"/>
+      <c r="B23" s="40" t="s">
+        <v>195</v>
+      </c>
+      <c r="C23" s="40"/>
+      <c r="D23" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="E23" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="F23" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="G23" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="H23" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I23" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+    </row>
+    <row r="24" spans="1:12" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="83"/>
+      <c r="B24" s="40" t="s">
+        <v>196</v>
+      </c>
+      <c r="C24" s="40"/>
+      <c r="D24" s="41" t="s">
+        <v>145</v>
+      </c>
+      <c r="E24" s="50" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="G24" s="41" t="s">
+        <v>160</v>
+      </c>
+      <c r="H24" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+    </row>
+    <row r="25" spans="1:12" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="83"/>
+      <c r="B25" s="40" t="s">
+        <v>197</v>
+      </c>
+      <c r="C25" s="40"/>
+      <c r="D25" s="41" t="s">
+        <v>146</v>
+      </c>
+      <c r="E25" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="G25" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="H25" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+    </row>
+    <row r="26" spans="1:12" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="83"/>
+      <c r="B26" s="40" t="s">
+        <v>198</v>
+      </c>
+      <c r="C26" s="40"/>
+      <c r="D26" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="J2" s="50"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="67"/>
-    </row>
-    <row r="3" spans="1:12" ht="239.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="78" t="s">
-        <v>157</v>
-      </c>
-      <c r="B3" s="49" t="s">
-        <v>148</v>
-      </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="50" t="s">
-        <v>158</v>
-      </c>
-      <c r="E3" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="50" t="s">
-        <v>150</v>
-      </c>
-      <c r="G3" s="50" t="s">
-        <v>159</v>
-      </c>
-      <c r="H3" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="39" t="s">
-        <v>160</v>
-      </c>
-      <c r="J3" s="50"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="67"/>
-    </row>
-    <row r="4" spans="1:12" ht="239.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="54"/>
-      <c r="B4" s="49" t="s">
-        <v>148</v>
-      </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="50" t="s">
-        <v>177</v>
-      </c>
-      <c r="E4" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="50" t="s">
-        <v>150</v>
-      </c>
-      <c r="G4" s="50" t="s">
+      <c r="E26" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="G26" s="41" t="s">
+        <v>153</v>
+      </c>
+      <c r="H26" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+    </row>
+    <row r="27" spans="1:12" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="84"/>
+      <c r="B27" s="40" t="s">
+        <v>199</v>
+      </c>
+      <c r="C27" s="40"/>
+      <c r="D27" s="41" t="s">
+        <v>147</v>
+      </c>
+      <c r="E27" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="41" t="s">
         <v>162</v>
       </c>
-      <c r="H4" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="39" t="s">
+      <c r="H27" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I27" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+    </row>
+    <row r="28" spans="1:12" ht="107.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="79" t="s">
+        <v>204</v>
+      </c>
+      <c r="B28" s="40" t="s">
+        <v>200</v>
+      </c>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41" t="s">
         <v>163</v>
       </c>
-      <c r="J4" s="50"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="36"/>
-    </row>
-    <row r="5" spans="1:12" ht="239.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="54"/>
-      <c r="B5" s="49" t="s">
-        <v>148</v>
-      </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="50" t="s">
-        <v>161</v>
-      </c>
-      <c r="E5" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="50" t="s">
-        <v>150</v>
-      </c>
-      <c r="G5" s="50" t="s">
-        <v>178</v>
-      </c>
-      <c r="H5" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="L5" s="77"/>
-    </row>
-    <row r="6" spans="1:12" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="54"/>
-      <c r="B6" s="49" t="s">
-        <v>148</v>
-      </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="50" t="s">
-        <v>179</v>
-      </c>
-      <c r="E6" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="50" t="s">
-        <v>150</v>
-      </c>
-      <c r="G6" s="50" t="s">
+      <c r="E28" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="G28" s="41" t="s">
         <v>164</v>
       </c>
-      <c r="H6" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="39" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="76"/>
-      <c r="B7" s="49" t="s">
-        <v>148</v>
-      </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="50" t="s">
+      <c r="H28" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" s="39" t="s">
+        <v>140</v>
+      </c>
+      <c r="J28" s="41"/>
+      <c r="K28" s="57"/>
+      <c r="L28" s="54"/>
+    </row>
+    <row r="29" spans="1:12" ht="147.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="80"/>
+      <c r="B29" s="40" t="s">
+        <v>201</v>
+      </c>
+      <c r="C29" s="40"/>
+      <c r="D29" s="77" t="s">
+        <v>165</v>
+      </c>
+      <c r="E29" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F29" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="G29" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="E7" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="50" t="s">
-        <v>150</v>
-      </c>
-      <c r="G7" s="50" t="s">
-        <v>165</v>
-      </c>
-      <c r="H7" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="39" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="76"/>
-      <c r="B8" s="49" t="s">
-        <v>148</v>
-      </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="50" t="s">
+      <c r="H29" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I29" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="J29" s="41"/>
+      <c r="K29" s="57"/>
+      <c r="L29" s="54"/>
+    </row>
+    <row r="30" spans="1:12" ht="85.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="81"/>
+      <c r="B30" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="C30" s="40"/>
+      <c r="D30" s="77" t="s">
+        <v>168</v>
+      </c>
+      <c r="E30" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F30" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="G30" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="H30" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I30" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="E8" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="50" t="s">
-        <v>150</v>
-      </c>
-      <c r="G8" s="50" t="s">
-        <v>170</v>
-      </c>
-      <c r="H8" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="39" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="76"/>
-      <c r="B9" s="49" t="s">
-        <v>148</v>
-      </c>
-      <c r="C9" s="49"/>
-      <c r="D9" s="50" t="s">
-        <v>168</v>
-      </c>
-      <c r="E9" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="50" t="s">
-        <v>150</v>
-      </c>
-      <c r="G9" s="50" t="s">
+      <c r="J30" s="41"/>
+      <c r="K30" s="57"/>
+      <c r="L30" s="54"/>
+    </row>
+    <row r="31" spans="1:12" ht="130.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" s="40" t="s">
+        <v>202</v>
+      </c>
+      <c r="C31" s="58"/>
+      <c r="D31" s="77" t="s">
+        <v>189</v>
+      </c>
+      <c r="E31" s="51" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="G31" s="41" t="s">
         <v>169</v>
       </c>
-      <c r="H9" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I9" s="39" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="76"/>
-      <c r="B10" s="49" t="s">
-        <v>148</v>
-      </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="50" t="s">
-        <v>172</v>
-      </c>
-      <c r="E10" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="50" t="s">
-        <v>150</v>
-      </c>
-      <c r="G10" s="50" t="s">
-        <v>171</v>
-      </c>
-      <c r="H10" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="39" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="76"/>
-      <c r="B11" s="49" t="s">
-        <v>148</v>
-      </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="50" t="s">
-        <v>173</v>
-      </c>
-      <c r="E11" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="50" t="s">
-        <v>150</v>
-      </c>
-      <c r="G11" s="50" t="s">
-        <v>174</v>
-      </c>
-      <c r="H11" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="39" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="221.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="76"/>
-      <c r="B12" s="49" t="s">
-        <v>148</v>
-      </c>
-      <c r="C12" s="49"/>
-      <c r="D12" s="50" t="s">
-        <v>175</v>
-      </c>
-      <c r="E12" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="50" t="s">
-        <v>176</v>
-      </c>
-      <c r="H12" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I12" s="39" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="233.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="53" t="s">
-        <v>180</v>
-      </c>
-      <c r="B13" s="49" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="D13" s="50" t="s">
-        <v>106</v>
-      </c>
-      <c r="E13" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="G13" s="50"/>
-      <c r="H13" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="39"/>
-      <c r="J13" s="50"/>
-      <c r="K13" s="70"/>
-      <c r="L13" s="67"/>
-    </row>
-    <row r="14" spans="1:12" ht="207.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="54"/>
-      <c r="B14" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="C14" s="49" t="s">
-        <v>94</v>
-      </c>
-      <c r="D14" s="50" t="s">
-        <v>108</v>
-      </c>
-      <c r="E14" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="G14" s="50"/>
-      <c r="H14" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="39"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="70"/>
-      <c r="L14" s="67"/>
-    </row>
-    <row r="15" spans="1:12" ht="249.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="53" t="s">
-        <v>109</v>
-      </c>
-      <c r="B15" s="49" t="s">
-        <v>110</v>
-      </c>
-      <c r="C15" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="50" t="s">
-        <v>111</v>
-      </c>
-      <c r="E15" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="G15" s="50"/>
-      <c r="H15" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I15" s="39"/>
-      <c r="J15" s="50"/>
-      <c r="K15" s="70"/>
-      <c r="L15" s="67"/>
-    </row>
-    <row r="16" spans="1:12" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="54"/>
-      <c r="B16" s="49" t="s">
-        <v>112</v>
-      </c>
-      <c r="C16" s="49" t="s">
-        <v>94</v>
-      </c>
-      <c r="D16" s="50" t="s">
-        <v>113</v>
-      </c>
-      <c r="E16" s="64" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="50" t="s">
-        <v>34</v>
-      </c>
-      <c r="G16" s="50"/>
-      <c r="H16" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I16" s="39"/>
-      <c r="J16" s="63"/>
-      <c r="K16" s="36"/>
-      <c r="L16" s="36"/>
-    </row>
-    <row r="17" spans="1:12" ht="130.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="58" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="49" t="s">
-        <v>153</v>
-      </c>
-      <c r="C17" s="71"/>
-      <c r="D17" s="50" t="s">
-        <v>154</v>
-      </c>
-      <c r="E17" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="G17" s="50" t="s">
-        <v>155</v>
-      </c>
-      <c r="H17" s="64" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17" s="72" t="s">
-        <v>156</v>
-      </c>
-      <c r="J17" s="63"/>
-      <c r="K17" s="70"/>
-      <c r="L17" s="67"/>
+      <c r="H31" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" s="77" t="s">
+        <v>188</v>
+      </c>
+      <c r="J31" s="50"/>
+      <c r="K31" s="57"/>
+      <c r="L31" s="54"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A18:A27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>
@@ -6821,10 +7416,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ADD30B2-DD71-45BD-B5D3-ECBDD8B20B47}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6832,78 +7427,174 @@
     <col min="1" max="1" width="25.28515625" customWidth="1"/>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="9" max="9" width="28.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
-        <v>87</v>
-      </c>
-      <c r="B1" s="44" t="s">
+    <row r="1" spans="1:12" ht="47.25" x14ac:dyDescent="0.2">
+      <c r="A1" s="85" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="86" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="E1" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="44" t="s">
+      <c r="F1" s="86" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="86" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="44" t="s">
+      <c r="H1" s="86" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="44" t="s">
+      <c r="I1" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="I1" s="44" t="s">
-        <v>90</v>
-      </c>
-      <c r="J1" s="44" t="s">
+      <c r="J1" s="86" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="86" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="40"/>
-    </row>
-    <row r="2" spans="1:11" ht="210" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="42" t="s">
-        <v>83</v>
-      </c>
-      <c r="G2" s="42" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" s="42" t="s">
-        <v>85</v>
-      </c>
-      <c r="I2" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="J2" s="42"/>
-      <c r="K2" s="40"/>
+    </row>
+    <row r="2" spans="1:12" ht="210" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="88" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="40" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="40"/>
+      <c r="D2" s="41" t="s">
+        <v>206</v>
+      </c>
+      <c r="E2" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="41" t="s">
+        <v>207</v>
+      </c>
+      <c r="H2" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="77" t="s">
+        <v>208</v>
+      </c>
+      <c r="J2" s="41"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="54"/>
+    </row>
+    <row r="3" spans="1:12" ht="210" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="89"/>
+      <c r="B3" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="40"/>
+      <c r="D3" s="41" t="s">
+        <v>214</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>217</v>
+      </c>
+      <c r="H3" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="77" t="s">
+        <v>218</v>
+      </c>
+      <c r="J3" s="41"/>
+      <c r="K3" s="57"/>
+      <c r="L3" s="54"/>
+    </row>
+    <row r="4" spans="1:12" ht="184.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="90" t="s">
+        <v>213</v>
+      </c>
+      <c r="B4" s="40" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" s="40"/>
+      <c r="D4" s="41" t="s">
+        <v>211</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="H4" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="77" t="s">
+        <v>212</v>
+      </c>
+      <c r="J4" s="41"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="54"/>
+    </row>
+    <row r="5" spans="1:12" ht="143.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="91"/>
+      <c r="B5" s="40" t="s">
+        <v>219</v>
+      </c>
+      <c r="C5" s="40"/>
+      <c r="D5" s="41" t="s">
+        <v>220</v>
+      </c>
+      <c r="E5" s="50" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="41" t="s">
+        <v>217</v>
+      </c>
+      <c r="H5" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="77" t="s">
+        <v>221</v>
+      </c>
+      <c r="J5" s="41"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Created Bug report document
</commit_message>
<xml_diff>
--- a/5- Testing/Test Cases.xlsx
+++ b/5- Testing/Test Cases.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="348">
   <si>
     <t>Assigned To</t>
   </si>
@@ -1448,6 +1448,10 @@
   </si>
   <si>
     <t>Percenatge of failed test cases</t>
+  </si>
+  <si>
+    <t>1- browser is available 
+2- Login as Admin successfully</t>
   </si>
 </sst>
 </file>
@@ -2302,6 +2306,27 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="32" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -2370,27 +2395,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="32" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2613,7 +2617,7 @@
   </sheetPr>
   <dimension ref="A1:AE991"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
@@ -2696,7 +2700,7 @@
       <c r="D2" s="83" t="s">
         <v>340</v>
       </c>
-      <c r="E2" s="110" t="s">
+      <c r="E2" s="85" t="s">
         <v>334</v>
       </c>
       <c r="F2" s="9">
@@ -2731,7 +2735,7 @@
       <c r="D3" s="83" t="s">
         <v>337</v>
       </c>
-      <c r="E3" s="110" t="s">
+      <c r="E3" s="85" t="s">
         <v>334</v>
       </c>
       <c r="F3" s="9">
@@ -2766,7 +2770,7 @@
       <c r="D4" s="83" t="s">
         <v>341</v>
       </c>
-      <c r="E4" s="110" t="s">
+      <c r="E4" s="85" t="s">
         <v>334</v>
       </c>
       <c r="F4" s="9">
@@ -2801,7 +2805,7 @@
       <c r="D5" s="83" t="s">
         <v>338</v>
       </c>
-      <c r="E5" s="110" t="s">
+      <c r="E5" s="85" t="s">
         <v>334</v>
       </c>
       <c r="F5" s="9">
@@ -2836,7 +2840,7 @@
       <c r="D6" s="83" t="s">
         <v>343</v>
       </c>
-      <c r="E6" s="110" t="s">
+      <c r="E6" s="85" t="s">
         <v>334</v>
       </c>
       <c r="F6" s="9">
@@ -2871,7 +2875,7 @@
       <c r="D7" s="83" t="s">
         <v>339</v>
       </c>
-      <c r="E7" s="110" t="s">
+      <c r="E7" s="85" t="s">
         <v>334</v>
       </c>
       <c r="F7" s="9">
@@ -2906,7 +2910,7 @@
       <c r="D8" s="83" t="s">
         <v>344</v>
       </c>
-      <c r="E8" s="110" t="s">
+      <c r="E8" s="85" t="s">
         <v>334</v>
       </c>
       <c r="F8" s="9">
@@ -2941,7 +2945,7 @@
       <c r="D9" s="83" t="s">
         <v>341</v>
       </c>
-      <c r="E9" s="110" t="s">
+      <c r="E9" s="85" t="s">
         <v>334</v>
       </c>
       <c r="F9" s="9">
@@ -2968,7 +2972,7 @@
       <c r="E10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="111">
+      <c r="F10" s="86">
         <f>SUM(F2:F9)</f>
         <v>80</v>
       </c>
@@ -2995,17 +2999,17 @@
     </row>
     <row r="11" spans="1:31" ht="61.2" customHeight="1">
       <c r="A11" s="10"/>
-      <c r="E11" s="112" t="s">
+      <c r="E11" s="87" t="s">
         <v>346</v>
       </c>
-      <c r="F11" s="115">
+      <c r="F11" s="90">
         <f>(H10/G10)*100</f>
         <v>97.5</v>
       </c>
     </row>
     <row r="12" spans="1:31" ht="74.400000000000006" customHeight="1">
       <c r="A12" s="10"/>
-      <c r="E12" s="113" t="s">
+      <c r="E12" s="88" t="s">
         <v>345</v>
       </c>
       <c r="F12" s="69">
@@ -3014,7 +3018,7 @@
       </c>
     </row>
     <row r="13" spans="1:31" ht="82.2" customHeight="1">
-      <c r="E13" s="114" t="s">
+      <c r="E13" s="89" t="s">
         <v>345</v>
       </c>
       <c r="F13" s="69">
@@ -5965,7 +5969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="95" workbookViewId="0">
+    <sheetView topLeftCell="D13" zoomScale="95" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C15"/>
     </sheetView>
   </sheetViews>
@@ -6023,7 +6027,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="207" customHeight="1">
-      <c r="A2" s="84"/>
+      <c r="A2" s="91"/>
       <c r="B2" s="30" t="s">
         <v>25</v>
       </c>
@@ -6057,7 +6061,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="175.5" customHeight="1">
-      <c r="A3" s="85"/>
+      <c r="A3" s="92"/>
       <c r="B3" s="30" t="s">
         <v>24</v>
       </c>
@@ -6091,8 +6095,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="124.2">
-      <c r="A4" s="85"/>
-      <c r="B4" s="88" t="s">
+      <c r="A4" s="92"/>
+      <c r="B4" s="95" t="s">
         <v>26</v>
       </c>
       <c r="C4" s="27" t="s">
@@ -6125,8 +6129,8 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="124.2">
-      <c r="A5" s="85"/>
-      <c r="B5" s="89"/>
+      <c r="A5" s="92"/>
+      <c r="B5" s="96"/>
       <c r="C5" s="27" t="s">
         <v>31</v>
       </c>
@@ -6157,8 +6161,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="124.2">
-      <c r="A6" s="85"/>
-      <c r="B6" s="89"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="96"/>
       <c r="C6" s="27" t="s">
         <v>111</v>
       </c>
@@ -6189,8 +6193,8 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="124.2">
-      <c r="A7" s="85"/>
-      <c r="B7" s="89"/>
+      <c r="A7" s="92"/>
+      <c r="B7" s="96"/>
       <c r="C7" s="27" t="s">
         <v>112</v>
       </c>
@@ -6221,8 +6225,8 @@
       </c>
     </row>
     <row r="8" spans="1:12" ht="124.2">
-      <c r="A8" s="85"/>
-      <c r="B8" s="89"/>
+      <c r="A8" s="92"/>
+      <c r="B8" s="96"/>
       <c r="C8" s="27" t="s">
         <v>113</v>
       </c>
@@ -6253,8 +6257,8 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="162" customHeight="1">
-      <c r="A9" s="85"/>
-      <c r="B9" s="89"/>
+      <c r="A9" s="92"/>
+      <c r="B9" s="96"/>
       <c r="C9" s="27" t="s">
         <v>114</v>
       </c>
@@ -6285,8 +6289,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="183" customHeight="1">
-      <c r="A10" s="85"/>
-      <c r="B10" s="90" t="s">
+      <c r="A10" s="92"/>
+      <c r="B10" s="97" t="s">
         <v>92</v>
       </c>
       <c r="C10" s="27" t="s">
@@ -6317,8 +6321,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="183" customHeight="1">
-      <c r="A11" s="85"/>
-      <c r="B11" s="91"/>
+      <c r="A11" s="92"/>
+      <c r="B11" s="98"/>
       <c r="C11" s="27" t="s">
         <v>118</v>
       </c>
@@ -6347,8 +6351,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="183" customHeight="1">
-      <c r="A12" s="85"/>
-      <c r="B12" s="91"/>
+      <c r="A12" s="92"/>
+      <c r="B12" s="98"/>
       <c r="C12" s="27" t="s">
         <v>119</v>
       </c>
@@ -6377,8 +6381,8 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="157.5" customHeight="1">
-      <c r="A13" s="85"/>
-      <c r="B13" s="92"/>
+      <c r="A13" s="92"/>
+      <c r="B13" s="99"/>
       <c r="C13" s="27" t="s">
         <v>120</v>
       </c>
@@ -6407,7 +6411,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="128.4">
-      <c r="A14" s="85"/>
+      <c r="A14" s="92"/>
       <c r="B14" s="31" t="s">
         <v>43</v>
       </c>
@@ -6441,7 +6445,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="83.4">
-      <c r="A15" s="86"/>
+      <c r="A15" s="93"/>
       <c r="B15" s="33" t="s">
         <v>51</v>
       </c>
@@ -6473,68 +6477,68 @@
       </c>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="85"/>
+      <c r="A16" s="92"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="85"/>
+      <c r="A17" s="92"/>
     </row>
     <row r="18" spans="1:4" ht="13.8">
-      <c r="A18" s="85"/>
+      <c r="A18" s="92"/>
       <c r="D18" s="44"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="85"/>
+      <c r="A19" s="92"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="85"/>
+      <c r="A20" s="92"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="85"/>
+      <c r="A21" s="92"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="85"/>
+      <c r="A22" s="92"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="85"/>
+      <c r="A23" s="92"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="85"/>
+      <c r="A24" s="92"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="85"/>
+      <c r="A25" s="92"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="85"/>
+      <c r="A26" s="92"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="85"/>
+      <c r="A27" s="92"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="85"/>
+      <c r="A28" s="92"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="85"/>
+      <c r="A29" s="92"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="85"/>
+      <c r="A30" s="92"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="85"/>
+      <c r="A31" s="92"/>
     </row>
     <row r="32" spans="1:4">
-      <c r="A32" s="85"/>
+      <c r="A32" s="92"/>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="85"/>
+      <c r="A33" s="92"/>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="85"/>
+      <c r="A34" s="92"/>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="85"/>
+      <c r="A35" s="92"/>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="87"/>
+      <c r="A36" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -6608,7 +6612,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="207.75" customHeight="1">
-      <c r="A2" s="84"/>
+      <c r="A2" s="91"/>
       <c r="B2" s="30" t="s">
         <v>25</v>
       </c>
@@ -6642,7 +6646,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="220.5" customHeight="1">
-      <c r="A3" s="85"/>
+      <c r="A3" s="92"/>
       <c r="B3" s="79" t="s">
         <v>51</v>
       </c>
@@ -6676,88 +6680,88 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="409.5" customHeight="1">
-      <c r="A4" s="85"/>
+      <c r="A4" s="92"/>
     </row>
     <row r="5" spans="1:12" ht="409.5" customHeight="1">
-      <c r="A5" s="85"/>
+      <c r="A5" s="92"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="85"/>
+      <c r="A6" s="92"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="85"/>
+      <c r="A7" s="92"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="85"/>
+      <c r="A8" s="92"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="85"/>
+      <c r="A9" s="92"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="85"/>
+      <c r="A10" s="92"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="85"/>
+      <c r="A11" s="92"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="85"/>
+      <c r="A12" s="92"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="85"/>
+      <c r="A13" s="92"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="85"/>
+      <c r="A14" s="92"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="85"/>
+      <c r="A15" s="92"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="85"/>
+      <c r="A16" s="92"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="85"/>
+      <c r="A17" s="92"/>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="85"/>
+      <c r="A18" s="92"/>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="85"/>
+      <c r="A19" s="92"/>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="85"/>
+      <c r="A20" s="92"/>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="85"/>
+      <c r="A21" s="92"/>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="85"/>
+      <c r="A22" s="92"/>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="85"/>
+      <c r="A23" s="92"/>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="85"/>
+      <c r="A24" s="92"/>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="85"/>
+      <c r="A25" s="92"/>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="85"/>
+      <c r="A26" s="92"/>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="85"/>
+      <c r="A27" s="92"/>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="85"/>
+      <c r="A28" s="92"/>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="85"/>
+      <c r="A29" s="92"/>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="85"/>
+      <c r="A30" s="92"/>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="87"/>
+      <c r="A31" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6828,7 +6832,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="213" customHeight="1">
-      <c r="A2" s="84"/>
+      <c r="A2" s="91"/>
       <c r="B2" s="18" t="s">
         <v>25</v>
       </c>
@@ -6862,91 +6866,91 @@
       </c>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="85"/>
+      <c r="A3" s="92"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="85"/>
+      <c r="A4" s="92"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="85"/>
+      <c r="A5" s="92"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="85"/>
+      <c r="A6" s="92"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="85"/>
+      <c r="A7" s="92"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="85"/>
+      <c r="A8" s="92"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="85"/>
+      <c r="A9" s="92"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="85"/>
+      <c r="A10" s="92"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="85"/>
+      <c r="A11" s="92"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="85"/>
+      <c r="A12" s="92"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="85"/>
+      <c r="A13" s="92"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="85"/>
+      <c r="A14" s="92"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="85"/>
+      <c r="A15" s="92"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="85"/>
+      <c r="A16" s="92"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="85"/>
+      <c r="A17" s="92"/>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="85"/>
+      <c r="A18" s="92"/>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="85"/>
+      <c r="A19" s="92"/>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="85"/>
+      <c r="A20" s="92"/>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="85"/>
+      <c r="A21" s="92"/>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="85"/>
+      <c r="A22" s="92"/>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="85"/>
+      <c r="A23" s="92"/>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="85"/>
+      <c r="A24" s="92"/>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="85"/>
+      <c r="A25" s="92"/>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="85"/>
+      <c r="A26" s="92"/>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="85"/>
+      <c r="A27" s="92"/>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="85"/>
+      <c r="A28" s="92"/>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="85"/>
+      <c r="A29" s="92"/>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" s="85"/>
+      <c r="A30" s="92"/>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" s="87"/>
+      <c r="A31" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -7014,7 +7018,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="179.25" customHeight="1">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="95" t="s">
         <v>67</v>
       </c>
       <c r="B2" s="69" t="s">
@@ -7047,7 +7051,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="148.5" customHeight="1">
-      <c r="A3" s="89"/>
+      <c r="A3" s="96"/>
       <c r="B3" s="69" t="s">
         <v>69</v>
       </c>
@@ -7078,7 +7082,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="135">
-      <c r="A4" s="88" t="s">
+      <c r="A4" s="95" t="s">
         <v>72</v>
       </c>
       <c r="B4" s="69" t="s">
@@ -7111,7 +7115,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="135">
-      <c r="A5" s="89"/>
+      <c r="A5" s="96"/>
       <c r="B5" s="69" t="s">
         <v>77</v>
       </c>
@@ -7142,7 +7146,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="135">
-      <c r="A6" s="88" t="s">
+      <c r="A6" s="95" t="s">
         <v>79</v>
       </c>
       <c r="B6" s="69" t="s">
@@ -7175,7 +7179,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="135">
-      <c r="A7" s="89"/>
+      <c r="A7" s="96"/>
       <c r="B7" s="69" t="s">
         <v>82</v>
       </c>
@@ -7206,7 +7210,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="135">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="95" t="s">
         <v>84</v>
       </c>
       <c r="B8" s="69" t="s">
@@ -7239,7 +7243,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="135">
-      <c r="A9" s="89"/>
+      <c r="A9" s="96"/>
       <c r="B9" s="69" t="s">
         <v>87</v>
       </c>
@@ -7372,7 +7376,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="239.25" customHeight="1">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="100" t="s">
         <v>127</v>
       </c>
       <c r="B3" s="69" t="s">
@@ -7405,7 +7409,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="239.25" customHeight="1">
-      <c r="A4" s="94"/>
+      <c r="A4" s="101"/>
       <c r="B4" s="69" t="s">
         <v>161</v>
       </c>
@@ -7436,7 +7440,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="239.25" customHeight="1">
-      <c r="A5" s="94"/>
+      <c r="A5" s="101"/>
       <c r="B5" s="69" t="s">
         <v>163</v>
       </c>
@@ -7467,7 +7471,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="221.25" customHeight="1">
-      <c r="A6" s="94"/>
+      <c r="A6" s="101"/>
       <c r="B6" s="69" t="s">
         <v>164</v>
       </c>
@@ -7684,7 +7688,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="233.25" customHeight="1">
-      <c r="A13" s="95" t="s">
+      <c r="A13" s="102" t="s">
         <v>139</v>
       </c>
       <c r="B13" s="69" t="s">
@@ -7717,7 +7721,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="207.75" customHeight="1">
-      <c r="A14" s="96"/>
+      <c r="A14" s="103"/>
       <c r="B14" s="69" t="s">
         <v>172</v>
       </c>
@@ -7845,7 +7849,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" ht="71.25" customHeight="1">
-      <c r="A18" s="100" t="s">
+      <c r="A18" s="107" t="s">
         <v>127</v>
       </c>
       <c r="B18" s="69" t="s">
@@ -7878,7 +7882,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" ht="90">
-      <c r="A19" s="101"/>
+      <c r="A19" s="108"/>
       <c r="B19" s="69" t="s">
         <v>180</v>
       </c>
@@ -7909,7 +7913,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="90">
-      <c r="A20" s="101"/>
+      <c r="A20" s="108"/>
       <c r="B20" s="69" t="s">
         <v>181</v>
       </c>
@@ -7940,7 +7944,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="90">
-      <c r="A21" s="101"/>
+      <c r="A21" s="108"/>
       <c r="B21" s="69" t="s">
         <v>182</v>
       </c>
@@ -7971,7 +7975,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="90">
-      <c r="A22" s="101"/>
+      <c r="A22" s="108"/>
       <c r="B22" s="69" t="s">
         <v>183</v>
       </c>
@@ -8002,7 +8006,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" ht="90">
-      <c r="A23" s="101"/>
+      <c r="A23" s="108"/>
       <c r="B23" s="69" t="s">
         <v>184</v>
       </c>
@@ -8033,7 +8037,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" ht="90">
-      <c r="A24" s="101"/>
+      <c r="A24" s="108"/>
       <c r="B24" s="69" t="s">
         <v>185</v>
       </c>
@@ -8064,7 +8068,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" ht="90">
-      <c r="A25" s="101"/>
+      <c r="A25" s="108"/>
       <c r="B25" s="69" t="s">
         <v>186</v>
       </c>
@@ -8095,7 +8099,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" ht="92.25" customHeight="1">
-      <c r="A26" s="101"/>
+      <c r="A26" s="108"/>
       <c r="B26" s="69" t="s">
         <v>187</v>
       </c>
@@ -8126,7 +8130,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="126" customHeight="1">
-      <c r="A27" s="102"/>
+      <c r="A27" s="109"/>
       <c r="B27" s="69" t="s">
         <v>188</v>
       </c>
@@ -8157,7 +8161,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" ht="107.25" customHeight="1">
-      <c r="A28" s="97" t="s">
+      <c r="A28" s="104" t="s">
         <v>193</v>
       </c>
       <c r="B28" s="69" t="s">
@@ -8190,7 +8194,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" ht="147.75" customHeight="1">
-      <c r="A29" s="98"/>
+      <c r="A29" s="105"/>
       <c r="B29" s="69" t="s">
         <v>190</v>
       </c>
@@ -8221,7 +8225,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="90">
-      <c r="A30" s="99"/>
+      <c r="A30" s="106"/>
       <c r="B30" s="69" t="s">
         <v>292</v>
       </c>
@@ -8300,8 +8304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -8355,7 +8359,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="210" customHeight="1">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="110" t="s">
         <v>198</v>
       </c>
       <c r="B2" s="27" t="s">
@@ -8388,7 +8392,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="210" customHeight="1">
-      <c r="A3" s="104"/>
+      <c r="A3" s="111"/>
       <c r="B3" s="27" t="s">
         <v>204</v>
       </c>
@@ -8417,7 +8421,7 @@
       <c r="K3" s="61"/>
     </row>
     <row r="4" spans="1:11" ht="184.5" customHeight="1">
-      <c r="A4" s="105" t="s">
+      <c r="A4" s="112" t="s">
         <v>201</v>
       </c>
       <c r="B4" s="27" t="s">
@@ -8448,7 +8452,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="143.25" customHeight="1">
-      <c r="A5" s="106"/>
+      <c r="A5" s="113"/>
       <c r="B5" s="27" t="s">
         <v>209</v>
       </c>
@@ -8459,7 +8463,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>52</v>
+        <v>347</v>
       </c>
       <c r="F5" s="28" t="s">
         <v>205</v>
@@ -8581,7 +8585,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="60">
-      <c r="A3" s="107" t="s">
+      <c r="A3" s="114" t="s">
         <v>127</v>
       </c>
       <c r="B3" s="27" t="s">
@@ -8614,7 +8618,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="55.2">
-      <c r="A4" s="108"/>
+      <c r="A4" s="115"/>
       <c r="B4" s="27" t="s">
         <v>220</v>
       </c>
@@ -8645,7 +8649,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="110.4">
-      <c r="A5" s="108"/>
+      <c r="A5" s="115"/>
       <c r="B5" s="27" t="s">
         <v>224</v>
       </c>
@@ -8676,7 +8680,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="55.2">
-      <c r="A6" s="108"/>
+      <c r="A6" s="115"/>
       <c r="B6" s="27" t="s">
         <v>228</v>
       </c>
@@ -8895,7 +8899,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="96.6">
-      <c r="A13" s="108" t="s">
+      <c r="A13" s="115" t="s">
         <v>139</v>
       </c>
       <c r="B13" s="27" t="s">
@@ -8928,7 +8932,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="110.4">
-      <c r="A14" s="108"/>
+      <c r="A14" s="115"/>
       <c r="B14" s="27" t="s">
         <v>256</v>
       </c>
@@ -8959,7 +8963,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="55.2">
-      <c r="A15" s="108" t="s">
+      <c r="A15" s="115" t="s">
         <v>84</v>
       </c>
       <c r="B15" s="27" t="s">
@@ -8992,7 +8996,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="69">
-      <c r="A16" s="108"/>
+      <c r="A16" s="115"/>
       <c r="B16" s="27" t="s">
         <v>263</v>
       </c>
@@ -9245,7 +9249,7 @@
         <v>321</v>
       </c>
       <c r="I2" s="70"/>
-      <c r="J2" s="109" t="s">
+      <c r="J2" s="84" t="s">
         <v>320</v>
       </c>
     </row>
@@ -9275,7 +9279,7 @@
         <v>326</v>
       </c>
       <c r="I3" s="70"/>
-      <c r="J3" s="109" t="s">
+      <c r="J3" s="84" t="s">
         <v>280</v>
       </c>
     </row>

</xml_diff>